<commit_message>
grouping by id agreement added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B01C96-2782-4776-8358-F6744D1FC011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC4A09-528A-4D43-AAA0-7ECC5F44F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" firstSheet="1" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" firstSheet="1" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="Com_Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$G$129</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$G$119</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$65</definedName>
     <definedName name="Адреса_банк_получателя">Export_Contract!$A$34</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$35</definedName>
@@ -43,74 +43,74 @@
     <definedName name="Доставка_условия">Export_Contract!$A$24</definedName>
     <definedName name="Инвойс">Com_Invoice!$D$4</definedName>
     <definedName name="Инвойс_Bl_массив">Com_Invoice!$B$16</definedName>
-    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$B$85</definedName>
+    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$B$75</definedName>
     <definedName name="Инвойс_банк_получателя">Com_Invoice!$B$44</definedName>
     <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$B$45</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$B$113</definedName>
-    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$B$112</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$B$103</definedName>
+    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$B$102</definedName>
     <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$B$46</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$B$114</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$B$104</definedName>
     <definedName name="Инвойс_всего">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_всего_п">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_дата">Com_Invoice!$B$10</definedName>
-    <definedName name="Инвойс_дата_п">Com_Invoice!$B$79</definedName>
+    <definedName name="Инвойс_дата_п">Com_Invoice!$B$69</definedName>
     <definedName name="Инвойс_декларация">Com_Invoice!$B$13</definedName>
-    <definedName name="Инвойс_декларация_п">Com_Invoice!$B$82</definedName>
+    <definedName name="Инвойс_декларация_п">Com_Invoice!$B$72</definedName>
     <definedName name="Инвойс_контракт">Com_Invoice!$D$11</definedName>
     <definedName name="Инвойс_контракт_дата">Com_Invoice!$D$12</definedName>
-    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$81</definedName>
-    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$80</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$71</definedName>
+    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$70</definedName>
     <definedName name="Инвойс_куда">Com_Invoice!$B$12</definedName>
-    <definedName name="Инвойс_куда_п">Com_Invoice!$B$81</definedName>
+    <definedName name="Инвойс_куда_п">Com_Invoice!$B$71</definedName>
     <definedName name="Инвойс_места">Com_Invoice!$D$16</definedName>
-    <definedName name="Инвойс_места_п">Com_Invoice!$D$85</definedName>
+    <definedName name="Инвойс_места_п">Com_Invoice!$D$75</definedName>
     <definedName name="Инвойс_откуда">Com_Invoice!$C$12</definedName>
-    <definedName name="Инвойс_откуда_п">Com_Invoice!$C$81</definedName>
-    <definedName name="Инвойс_п">Com_Invoice!$D$73</definedName>
+    <definedName name="Инвойс_откуда_п">Com_Invoice!$C$71</definedName>
+    <definedName name="Инвойс_п">Com_Invoice!$D$63</definedName>
     <definedName name="Инвойс_подвал_всего">Com_Invoice!$D$42</definedName>
-    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$110</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$100</definedName>
     <definedName name="Инвойс_подвал_сумма">Com_Invoice!$F$42</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$F$110</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$F$100</definedName>
     <definedName name="Инвойс_подписант">Com_Invoice!$D$44</definedName>
-    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$112</definedName>
+    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$102</definedName>
     <definedName name="Инвойс_покупатель">Com_Invoice!$D$7</definedName>
     <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$D$8</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$77</definedName>
-    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$76</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$67</definedName>
+    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$66</definedName>
     <definedName name="Инвойс_получатель">Com_Invoice!$B$7</definedName>
     <definedName name="Инвойс_получатель_адрес">Com_Invoice!$B$8</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$B$77</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$B$67</definedName>
     <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$B$47</definedName>
-    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$B$115</definedName>
-    <definedName name="Инвойс_получатель_п">Com_Invoice!$B$76</definedName>
+    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$B$105</definedName>
+    <definedName name="Инвойс_получатель_п">Com_Invoice!$B$66</definedName>
     <definedName name="Инвойс_получатель_счет">Com_Invoice!$B$48</definedName>
-    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$B$116</definedName>
+    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$B$106</definedName>
     <definedName name="Инвойс_продавец">Com_Invoice!$B$4</definedName>
     <definedName name="Инвойс_продавец_адрес">Com_Invoice!$B$5</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$B$74</definedName>
-    <definedName name="Инвойс_продавец_п">Com_Invoice!$B$73</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$B$64</definedName>
+    <definedName name="Инвойс_продавец_п">Com_Invoice!$B$63</definedName>
     <definedName name="Инвойс_продукт">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_продукт_п">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_соглашение">Com_Invoice!$D$10</definedName>
-    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$79</definedName>
+    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$69</definedName>
     <definedName name="Инвойс_судно">Com_Invoice!$B$39</definedName>
-    <definedName name="Инвойс_судно_п">Com_Invoice!$B$107</definedName>
+    <definedName name="Инвойс_судно_п">Com_Invoice!$B$97</definedName>
     <definedName name="Инвойс_сумма">Com_Invoice!$F$16</definedName>
-    <definedName name="Инвойс_сумма_п">Com_Invoice!$F$85</definedName>
+    <definedName name="Инвойс_сумма_п">Com_Invoice!$F$75</definedName>
     <definedName name="Инвойс_транспорт">Com_Invoice!$C$10</definedName>
-    <definedName name="Инвойс_транспорт_п">Com_Invoice!$C$79</definedName>
+    <definedName name="Инвойс_транспорт_п">Com_Invoice!$C$69</definedName>
     <definedName name="Инвойс_упаковка">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_упаковка_п">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_условия">Com_Invoice!$D$14</definedName>
-    <definedName name="Инвойс_условия_п">Com_Invoice!$D$83</definedName>
+    <definedName name="Инвойс_условия_п">Com_Invoice!$D$73</definedName>
     <definedName name="Инвойс_цена">Com_Invoice!$E$16</definedName>
-    <definedName name="Инвойс_цена_п">Com_Invoice!$E$85</definedName>
+    <definedName name="Инвойс_цена_п">Com_Invoice!$E$75</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="МСЦ">Com_Invoice!$E$4</definedName>
-    <definedName name="МСЦ_п">Com_Invoice!$E$73</definedName>
+    <definedName name="МСЦ_п">Com_Invoice!$E$63</definedName>
     <definedName name="МСЦ_сертификат">Com_Invoice!$F$4</definedName>
-    <definedName name="МСЦ_сертификат_п">Com_Invoice!$F$73</definedName>
+    <definedName name="МСЦ_сертификат_п">Com_Invoice!$F$63</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
     <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
@@ -2285,10 +2285,10 @@
     <tabColor theme="9" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Y129"/>
+  <dimension ref="A2:Y119"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2895,305 +2895,353 @@
       <c r="F48" s="66"/>
       <c r="G48" s="50"/>
     </row>
-    <row r="49" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
     </row>
-    <row r="50" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
     </row>
-    <row r="51" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="44"/>
       <c r="C51" s="44"/>
     </row>
-    <row r="52" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="44"/>
       <c r="C52" s="44"/>
     </row>
-    <row r="53" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
     </row>
-    <row r="54" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
     </row>
-    <row r="55" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="44"/>
       <c r="C55" s="44"/>
     </row>
-    <row r="56" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="44"/>
       <c r="C56" s="44"/>
     </row>
-    <row r="57" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="44"/>
       <c r="C57" s="44"/>
     </row>
-    <row r="58" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="44"/>
       <c r="C58" s="44"/>
     </row>
-    <row r="59" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="44"/>
       <c r="C59" s="44"/>
     </row>
-    <row r="60" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="44"/>
       <c r="C60" s="44"/>
     </row>
-    <row r="61" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
-    </row>
-    <row r="62" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="44"/>
-      <c r="C62" s="44"/>
-    </row>
-    <row r="63" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="44"/>
+    <row r="61" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="B61" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="82"/>
+      <c r="F61" s="82"/>
+    </row>
+    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="51"/>
+      <c r="B62" s="84" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="84"/>
+      <c r="D62" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="E62" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="50"/>
+    </row>
+    <row r="63" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="51"/>
+      <c r="B63" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="C63" s="44"/>
-    </row>
-    <row r="64" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B64" s="44"/>
-      <c r="C64" s="44"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="44"/>
-      <c r="C65" s="44"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B66" s="44"/>
-      <c r="C66" s="44"/>
-    </row>
-    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B67" s="44"/>
-      <c r="C67" s="44"/>
-    </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B68" s="44"/>
-      <c r="C68" s="44"/>
-    </row>
-    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B69" s="44"/>
-      <c r="C69" s="44"/>
-    </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B70" s="44"/>
-      <c r="C70" s="44"/>
-    </row>
-    <row r="71" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="B71" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="C71" s="82"/>
-      <c r="D71" s="82"/>
-      <c r="E71" s="82"/>
-      <c r="F71" s="82"/>
-    </row>
-    <row r="72" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D63" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="50"/>
+    </row>
+    <row r="64" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="51"/>
+      <c r="B64" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="68"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="50"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A65" s="51"/>
+      <c r="B65" s="88" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" s="84"/>
+      <c r="D65" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" s="53"/>
+      <c r="F65" s="54"/>
+      <c r="G65" s="50"/>
+    </row>
+    <row r="66" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="51"/>
+      <c r="B66" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="47"/>
+      <c r="D66" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" s="44"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="50"/>
+    </row>
+    <row r="67" spans="1:15" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="51"/>
+      <c r="B67" s="110" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="110"/>
+      <c r="D67" s="109" t="s">
+        <v>151</v>
+      </c>
+      <c r="E67" s="110"/>
+      <c r="F67" s="111"/>
+      <c r="G67" s="50"/>
+    </row>
+    <row r="68" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="51"/>
+      <c r="B68" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" s="53"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="50"/>
+    </row>
+    <row r="69" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="51"/>
+      <c r="B69" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="60"/>
+      <c r="F69" s="61"/>
+      <c r="G69" s="50"/>
+    </row>
+    <row r="70" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="51"/>
+      <c r="B70" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" s="90"/>
+      <c r="D70" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" s="44"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="50"/>
+    </row>
+    <row r="71" spans="1:15" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="51"/>
+      <c r="B71" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="E71" s="68"/>
+      <c r="F71" s="69"/>
+      <c r="G71" s="50"/>
+    </row>
+    <row r="72" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="51"/>
-      <c r="B72" s="84" t="s">
-        <v>46</v>
-      </c>
-      <c r="C72" s="84"/>
-      <c r="D72" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="E72" s="85" t="s">
-        <v>3</v>
-      </c>
-      <c r="F72" s="86" t="s">
-        <v>4</v>
-      </c>
+      <c r="B72" t="s">
+        <v>130</v>
+      </c>
+      <c r="D72" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="E72" s="53"/>
+      <c r="F72" s="54"/>
       <c r="G72" s="50"/>
     </row>
-    <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" s="51"/>
-      <c r="B73" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C73" s="44"/>
-      <c r="D73" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" s="72" t="s">
-        <v>8</v>
-      </c>
+      <c r="D73" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73" s="68"/>
+      <c r="F73" s="69"/>
       <c r="G73" s="50"/>
     </row>
-    <row r="74" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="51"/>
-      <c r="B74" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="C74" s="68"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="51"/>
+      <c r="B74" s="91" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="D74" s="92" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F74" s="93" t="s">
+        <v>62</v>
+      </c>
       <c r="G74" s="50"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:15" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="51"/>
-      <c r="B75" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="C75" s="84"/>
-      <c r="D75" s="52" t="s">
-        <v>146</v>
-      </c>
-      <c r="E75" s="53"/>
-      <c r="F75" s="54"/>
+      <c r="B75" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="C75" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="E75" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="F75" s="49" t="s">
+        <v>64</v>
+      </c>
       <c r="G75" s="50"/>
     </row>
-    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="51"/>
-      <c r="B76" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="47"/>
-      <c r="D76" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="E76" s="44"/>
-      <c r="F76" s="56"/>
+      <c r="B76" s="70"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="70"/>
+      <c r="E76" s="70"/>
+      <c r="F76" s="49"/>
       <c r="G76" s="50"/>
     </row>
-    <row r="77" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="51"/>
-      <c r="B77" s="110" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" s="110"/>
-      <c r="D77" s="109" t="s">
-        <v>151</v>
-      </c>
-      <c r="E77" s="110"/>
-      <c r="F77" s="111"/>
+      <c r="B77" s="70"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="70"/>
+      <c r="E77" s="70"/>
+      <c r="F77" s="49"/>
       <c r="G77" s="50"/>
     </row>
-    <row r="78" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="51"/>
-      <c r="B78" s="90" t="s">
-        <v>52</v>
-      </c>
-      <c r="C78" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="D78" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="E78" s="53"/>
-      <c r="F78" s="54"/>
+      <c r="B78" s="70"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="70"/>
+      <c r="E78" s="70"/>
+      <c r="F78" s="49"/>
       <c r="G78" s="50"/>
     </row>
-    <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A79" s="51"/>
-      <c r="B79" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C79" s="89" t="s">
-        <v>55</v>
-      </c>
-      <c r="D79" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E79" s="60"/>
-      <c r="F79" s="61"/>
+      <c r="E79" s="70"/>
+      <c r="F79" s="49"/>
       <c r="G79" s="50"/>
     </row>
-    <row r="80" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="51"/>
-      <c r="B80" s="90" t="s">
-        <v>57</v>
-      </c>
-      <c r="C80" s="90"/>
-      <c r="D80" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="E80" s="44"/>
-      <c r="F80" s="56"/>
+      <c r="B80" s="70"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="70"/>
+      <c r="E80" s="70"/>
+      <c r="F80" s="49"/>
       <c r="G80" s="50"/>
-    </row>
-    <row r="81" spans="1:15" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O80" s="94"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="51"/>
-      <c r="B81" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="C81" s="68" t="s">
-        <v>151</v>
-      </c>
-      <c r="D81" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="E81" s="68"/>
-      <c r="F81" s="69"/>
+      <c r="B81" s="70"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="70"/>
+      <c r="F81" s="49"/>
       <c r="G81" s="50"/>
     </row>
-    <row r="82" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="51"/>
-      <c r="B82" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="E82" s="53"/>
-      <c r="F82" s="54"/>
+      <c r="B82" s="70"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="70"/>
+      <c r="E82" s="70"/>
+      <c r="F82" s="49"/>
       <c r="G82" s="50"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="51"/>
-      <c r="D83" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E83" s="68"/>
-      <c r="F83" s="69"/>
+      <c r="B83" s="70"/>
+      <c r="C83" s="70"/>
+      <c r="D83" s="70"/>
+      <c r="E83" s="70"/>
+      <c r="F83" s="49"/>
       <c r="G83" s="50"/>
     </row>
-    <row r="84" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="51"/>
-      <c r="B84" s="91" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="91" t="s">
-        <v>133</v>
-      </c>
-      <c r="D84" s="92" t="s">
-        <v>154</v>
-      </c>
-      <c r="E84" s="91" t="s">
-        <v>156</v>
-      </c>
-      <c r="F84" s="93" t="s">
-        <v>62</v>
-      </c>
+      <c r="B84" s="70"/>
+      <c r="C84" s="70"/>
+      <c r="D84" s="70"/>
+      <c r="E84" s="70"/>
+      <c r="F84" s="49"/>
       <c r="G84" s="50"/>
     </row>
-    <row r="85" spans="1:15" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="51"/>
-      <c r="B85" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="C85" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="D85" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="E85" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="F85" s="49" t="s">
-        <v>64</v>
-      </c>
+      <c r="B85" s="70"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="70"/>
+      <c r="E85" s="70"/>
+      <c r="F85" s="49"/>
       <c r="G85" s="50"/>
     </row>
-    <row r="86" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="51"/>
       <c r="B86" s="70"/>
       <c r="C86" s="70"/>
@@ -3202,7 +3250,7 @@
       <c r="F86" s="49"/>
       <c r="G86" s="50"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="51"/>
       <c r="B87" s="70"/>
       <c r="C87" s="70"/>
@@ -3211,7 +3259,7 @@
       <c r="F87" s="49"/>
       <c r="G87" s="50"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="51"/>
       <c r="B88" s="70"/>
       <c r="C88" s="70"/>
@@ -3220,13 +3268,16 @@
       <c r="F88" s="49"/>
       <c r="G88" s="50"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="51"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="70"/>
       <c r="E89" s="70"/>
       <c r="F89" s="49"/>
       <c r="G89" s="50"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="51"/>
       <c r="B90" s="70"/>
       <c r="C90" s="70"/>
@@ -3234,9 +3285,8 @@
       <c r="E90" s="70"/>
       <c r="F90" s="49"/>
       <c r="G90" s="50"/>
-      <c r="O90" s="94"/>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="51"/>
       <c r="B91" s="70"/>
       <c r="C91" s="70"/>
@@ -3245,7 +3295,7 @@
       <c r="F91" s="49"/>
       <c r="G91" s="50"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="51"/>
       <c r="B92" s="70"/>
       <c r="C92" s="70"/>
@@ -3254,7 +3304,7 @@
       <c r="F92" s="49"/>
       <c r="G92" s="50"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="51"/>
       <c r="B93" s="70"/>
       <c r="C93" s="70"/>
@@ -3263,7 +3313,7 @@
       <c r="F93" s="49"/>
       <c r="G93" s="50"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="51"/>
       <c r="B94" s="70"/>
       <c r="C94" s="70"/>
@@ -3272,7 +3322,7 @@
       <c r="F94" s="49"/>
       <c r="G94" s="50"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="51"/>
       <c r="B95" s="70"/>
       <c r="C95" s="70"/>
@@ -3281,237 +3331,147 @@
       <c r="F95" s="49"/>
       <c r="G95" s="50"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="51"/>
-      <c r="B96" s="70"/>
-      <c r="C96" s="70"/>
-      <c r="D96" s="70"/>
-      <c r="E96" s="70"/>
-      <c r="F96" s="49"/>
+      <c r="B96" s="45"/>
+      <c r="C96" s="45"/>
+      <c r="D96" s="45"/>
+      <c r="E96" s="77"/>
+      <c r="F96" s="62"/>
       <c r="G96" s="50"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="51"/>
-      <c r="B97" s="70"/>
-      <c r="C97" s="70"/>
-      <c r="D97" s="70"/>
-      <c r="E97" s="70"/>
-      <c r="F97" s="49"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="6"/>
       <c r="G97" s="50"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="51"/>
-      <c r="B98" s="70"/>
-      <c r="C98" s="70"/>
-      <c r="D98" s="70"/>
-      <c r="E98" s="70"/>
-      <c r="F98" s="49"/>
+      <c r="B98" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="6"/>
       <c r="G98" s="50"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="51"/>
-      <c r="B99" s="70"/>
-      <c r="C99" s="70"/>
-      <c r="D99" s="70"/>
-      <c r="E99" s="70"/>
-      <c r="F99" s="49"/>
+      <c r="B99" s="74" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" s="74"/>
+      <c r="D99" s="74"/>
+      <c r="E99" s="74"/>
+      <c r="F99" s="75"/>
       <c r="G99" s="50"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="51"/>
-      <c r="B100" s="70"/>
-      <c r="C100" s="70"/>
-      <c r="D100" s="70"/>
-      <c r="E100" s="70"/>
-      <c r="F100" s="49"/>
+      <c r="B100" s="39"/>
+      <c r="C100" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="D100" s="104" t="s">
+        <v>139</v>
+      </c>
+      <c r="E100" s="77"/>
+      <c r="F100" s="78" t="s">
+        <v>140</v>
+      </c>
       <c r="G100" s="50"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="51"/>
-      <c r="B101" s="70"/>
-      <c r="C101" s="70"/>
-      <c r="D101" s="70"/>
-      <c r="E101" s="70"/>
-      <c r="F101" s="49"/>
+      <c r="B101" s="114" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="114"/>
+      <c r="D101" s="114"/>
+      <c r="E101" s="77"/>
+      <c r="F101" s="62"/>
       <c r="G101" s="50"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="51"/>
-      <c r="B102" s="70"/>
-      <c r="C102" s="70"/>
-      <c r="D102" s="70"/>
-      <c r="E102" s="70"/>
-      <c r="F102" s="49"/>
+      <c r="B102" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="C102" s="80"/>
+      <c r="D102" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="E102" s="53"/>
+      <c r="F102" s="54"/>
       <c r="G102" s="50"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="51"/>
-      <c r="B103" s="70"/>
-      <c r="C103" s="70"/>
-      <c r="D103" s="70"/>
-      <c r="E103" s="70"/>
-      <c r="F103" s="49"/>
+      <c r="B103" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="47"/>
+      <c r="D103" s="50"/>
+      <c r="F103" s="51"/>
       <c r="G103" s="50"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="51"/>
-      <c r="B104" s="70"/>
-      <c r="C104" s="70"/>
-      <c r="D104" s="70"/>
-      <c r="E104" s="70"/>
-      <c r="F104" s="49"/>
+      <c r="B104" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C104" s="47"/>
+      <c r="D104" s="50"/>
+      <c r="F104" s="51"/>
       <c r="G104" s="50"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="51"/>
-      <c r="B105" s="70"/>
-      <c r="C105" s="70"/>
-      <c r="D105" s="70"/>
-      <c r="E105" s="70"/>
-      <c r="F105" s="49"/>
+      <c r="B105" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C105" s="47"/>
+      <c r="D105" s="50"/>
+      <c r="F105" s="51"/>
       <c r="G105" s="50"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="51"/>
-      <c r="B106" s="45"/>
-      <c r="C106" s="45"/>
-      <c r="D106" s="45"/>
-      <c r="E106" s="77"/>
-      <c r="F106" s="62"/>
+      <c r="B106" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C106" s="68"/>
+      <c r="D106" s="81"/>
+      <c r="E106" s="65"/>
+      <c r="F106" s="66"/>
       <c r="G106" s="50"/>
     </row>
-    <row r="107" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A107" s="51"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="6"/>
-      <c r="G107" s="50"/>
-    </row>
-    <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A108" s="51"/>
-      <c r="B108" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="50"/>
-    </row>
-    <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="51"/>
-      <c r="B109" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="C109" s="74"/>
-      <c r="D109" s="74"/>
-      <c r="E109" s="74"/>
-      <c r="F109" s="75"/>
-      <c r="G109" s="50"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A110" s="51"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="76" t="s">
-        <v>149</v>
-      </c>
-      <c r="D110" s="104" t="s">
-        <v>139</v>
-      </c>
-      <c r="E110" s="77"/>
-      <c r="F110" s="78" t="s">
-        <v>140</v>
-      </c>
-      <c r="G110" s="50"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A111" s="51"/>
-      <c r="B111" s="114" t="s">
-        <v>38</v>
-      </c>
-      <c r="C111" s="114"/>
-      <c r="D111" s="114"/>
-      <c r="E111" s="77"/>
-      <c r="F111" s="62"/>
-      <c r="G111" s="50"/>
-    </row>
-    <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="51"/>
-      <c r="B112" s="80" t="s">
-        <v>39</v>
-      </c>
-      <c r="C112" s="80"/>
-      <c r="D112" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="E112" s="53"/>
-      <c r="F112" s="54"/>
-      <c r="G112" s="50"/>
-    </row>
-    <row r="113" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A113" s="51"/>
-      <c r="B113" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C113" s="47"/>
-      <c r="D113" s="50"/>
-      <c r="F113" s="51"/>
-      <c r="G113" s="50"/>
-    </row>
-    <row r="114" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A114" s="51"/>
-      <c r="B114" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C114" s="47"/>
-      <c r="D114" s="50"/>
-      <c r="F114" s="51"/>
-      <c r="G114" s="50"/>
-    </row>
-    <row r="115" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A115" s="51"/>
-      <c r="B115" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C115" s="47"/>
-      <c r="D115" s="50"/>
-      <c r="F115" s="51"/>
-      <c r="G115" s="50"/>
-    </row>
-    <row r="116" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A116" s="51"/>
-      <c r="B116" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="C116" s="68"/>
-      <c r="D116" s="81"/>
-      <c r="E116" s="65"/>
-      <c r="F116" s="66"/>
-      <c r="G116" s="50"/>
-    </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="129" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="113" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="114" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="115" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="116" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="117" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="118" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="119" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:F67"/>
     <mergeCell ref="B43:D43"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
addresses added in tmp
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC4A09-528A-4D43-AAA0-7ECC5F44F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78B50B8-7DAB-486F-B3DC-20EB446342FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" firstSheet="1" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" firstSheet="1" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="Com_Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$G$119</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$G$116</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$65</definedName>
     <definedName name="Адреса_банк_получателя">Export_Contract!$A$34</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$35</definedName>
@@ -1564,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A36" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2285,10 +2285,10 @@
     <tabColor theme="9" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Y119"/>
+  <dimension ref="A2:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A83" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2937,7 +2937,6 @@
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="44"/>
-      <c r="C59" s="44"/>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="44"/>
@@ -3440,7 +3439,7 @@
       <c r="F105" s="51"/>
       <c r="G105" s="50"/>
     </row>
-    <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="51"/>
       <c r="B106" s="68" t="s">
         <v>44</v>
@@ -3451,19 +3450,6 @@
       <c r="F106" s="66"/>
       <c r="G106" s="50"/>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="113" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="114" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="115" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="116" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="117" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="118" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="119" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B8:C8"/>
@@ -3477,5 +3463,8 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="57" max="6" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
initComInvoiceTerms fn added, invoice init refactored
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E532B-6927-46EB-BA31-E5414D590A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEDC8F7-6C38-4F31-865A-C166D17BCEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" firstSheet="1" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -64,8 +64,6 @@
     <definedName name="Инвойс_куда_п">Com_Invoice!$B$71</definedName>
     <definedName name="Инвойс_места">Com_Invoice!$D$16</definedName>
     <definedName name="Инвойс_места_п">Com_Invoice!$D$75</definedName>
-    <definedName name="Инвойс_откуда">Com_Invoice!$C$12</definedName>
-    <definedName name="Инвойс_откуда_п">Com_Invoice!$C$71</definedName>
     <definedName name="Инвойс_п">Com_Invoice!$D$63</definedName>
     <definedName name="Инвойс_подвал_всего">Com_Invoice!$D$42</definedName>
     <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$100</definedName>
@@ -156,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="158">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -1564,8 +1562,8 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A36" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A27" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2287,8 +2285,8 @@
   </sheetPr>
   <dimension ref="A2:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A66" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2462,9 +2460,7 @@
       <c r="B12" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="64" t="s">
-        <v>147</v>
-      </c>
+      <c r="C12" s="64"/>
       <c r="D12" s="67" t="s">
         <v>24</v>
       </c>
@@ -3083,9 +3079,7 @@
       <c r="B71" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="C71" s="68" t="s">
-        <v>147</v>
-      </c>
+      <c r="C71" s="68"/>
       <c r="D71" s="67" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
minor fixes + deliveryFCA refactored + tmp refactored
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -8,107 +8,108 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEDC8F7-6C38-4F31-865A-C166D17BCEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3C2B6B-89BB-4773-9D27-84F622AD8F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16394" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="Com_Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$G$116</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$65</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$A$34</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$35</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$A$36</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$A$48</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$A$40</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$A$41</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$A$42</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$A$44</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$A$43</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$A$45</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$A$46</definedName>
-    <definedName name="Адреса_покупатель_заголовок">Export_Contract!$A$39</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$A$47</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$A$37</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$A$38</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$A$32</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$A$33</definedName>
-    <definedName name="Адреса_продавец_заголовок">Export_Contract!$A$31</definedName>
-    <definedName name="Адреса_сторон_заголовок">Export_Contract!$A$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$G$123</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$62</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$A$31</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$32</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$A$33</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$A$45</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$A$37</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$A$38</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$A$39</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$A$41</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$A$40</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$A$42</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$A$43</definedName>
+    <definedName name="Адреса_покупатель_заголовок">Export_Contract!$A$36</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$A$44</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$A$34</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$A$35</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$A$29</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$A$30</definedName>
+    <definedName name="Адреса_продавец_заголовок">Export_Contract!$A$28</definedName>
+    <definedName name="Адреса_сторон_заголовок">Export_Contract!$A$27</definedName>
+    <definedName name="Доставка_дата">Export_Contract!$A$26</definedName>
     <definedName name="Доставка_заголовок">Export_Contract!$A$23</definedName>
-    <definedName name="Доставка_порт">Export_Contract!$A$25</definedName>
+    <definedName name="Доставка_приемка">Export_Contract!$A$25</definedName>
     <definedName name="Доставка_условия">Export_Contract!$A$24</definedName>
     <definedName name="Инвойс">Com_Invoice!$D$4</definedName>
     <definedName name="Инвойс_Bl_массив">Com_Invoice!$B$16</definedName>
-    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$B$75</definedName>
+    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$B$82</definedName>
     <definedName name="Инвойс_банк_получателя">Com_Invoice!$B$44</definedName>
     <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$B$45</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$B$103</definedName>
-    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$B$102</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$B$110</definedName>
+    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$B$109</definedName>
     <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$B$46</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$B$104</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$B$111</definedName>
     <definedName name="Инвойс_всего">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_всего_п">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_дата">Com_Invoice!$B$10</definedName>
-    <definedName name="Инвойс_дата_п">Com_Invoice!$B$69</definedName>
+    <definedName name="Инвойс_дата_п">Com_Invoice!$B$76</definedName>
     <definedName name="Инвойс_декларация">Com_Invoice!$B$13</definedName>
-    <definedName name="Инвойс_декларация_п">Com_Invoice!$B$72</definedName>
+    <definedName name="Инвойс_декларация_п">Com_Invoice!$B$79</definedName>
     <definedName name="Инвойс_контракт">Com_Invoice!$D$11</definedName>
     <definedName name="Инвойс_контракт_дата">Com_Invoice!$D$12</definedName>
-    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$71</definedName>
-    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$70</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$78</definedName>
+    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$77</definedName>
     <definedName name="Инвойс_куда">Com_Invoice!$B$12</definedName>
-    <definedName name="Инвойс_куда_п">Com_Invoice!$B$71</definedName>
+    <definedName name="Инвойс_куда_п">Com_Invoice!$B$78</definedName>
     <definedName name="Инвойс_места">Com_Invoice!$D$16</definedName>
-    <definedName name="Инвойс_места_п">Com_Invoice!$D$75</definedName>
-    <definedName name="Инвойс_п">Com_Invoice!$D$63</definedName>
+    <definedName name="Инвойс_места_п">Com_Invoice!$D$82</definedName>
+    <definedName name="Инвойс_п">Com_Invoice!$D$70</definedName>
     <definedName name="Инвойс_подвал_всего">Com_Invoice!$D$42</definedName>
-    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$100</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$107</definedName>
     <definedName name="Инвойс_подвал_сумма">Com_Invoice!$F$42</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$F$100</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$F$107</definedName>
     <definedName name="Инвойс_подписант">Com_Invoice!$D$44</definedName>
-    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$102</definedName>
+    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$109</definedName>
     <definedName name="Инвойс_покупатель">Com_Invoice!$D$7</definedName>
     <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$D$8</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$67</definedName>
-    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$66</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$74</definedName>
+    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$73</definedName>
     <definedName name="Инвойс_получатель">Com_Invoice!$B$7</definedName>
     <definedName name="Инвойс_получатель_адрес">Com_Invoice!$B$8</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$B$67</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$B$74</definedName>
     <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$B$47</definedName>
-    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$B$105</definedName>
-    <definedName name="Инвойс_получатель_п">Com_Invoice!$B$66</definedName>
+    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$B$112</definedName>
+    <definedName name="Инвойс_получатель_п">Com_Invoice!$B$73</definedName>
     <definedName name="Инвойс_получатель_счет">Com_Invoice!$B$48</definedName>
-    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$B$106</definedName>
+    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$B$113</definedName>
     <definedName name="Инвойс_продавец">Com_Invoice!$B$4</definedName>
     <definedName name="Инвойс_продавец_адрес">Com_Invoice!$B$5</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$B$64</definedName>
-    <definedName name="Инвойс_продавец_п">Com_Invoice!$B$63</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$B$71</definedName>
+    <definedName name="Инвойс_продавец_п">Com_Invoice!$B$70</definedName>
     <definedName name="Инвойс_продукт">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_продукт_п">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_соглашение">Com_Invoice!$D$10</definedName>
-    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$69</definedName>
+    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$76</definedName>
     <definedName name="Инвойс_судно">Com_Invoice!$B$39</definedName>
-    <definedName name="Инвойс_судно_п">Com_Invoice!$B$97</definedName>
+    <definedName name="Инвойс_судно_п">Com_Invoice!$B$104</definedName>
     <definedName name="Инвойс_сумма">Com_Invoice!$F$16</definedName>
-    <definedName name="Инвойс_сумма_п">Com_Invoice!$F$75</definedName>
+    <definedName name="Инвойс_сумма_п">Com_Invoice!$F$82</definedName>
     <definedName name="Инвойс_транспорт">Com_Invoice!$C$10</definedName>
-    <definedName name="Инвойс_транспорт_п">Com_Invoice!$C$69</definedName>
+    <definedName name="Инвойс_транспорт_п">Com_Invoice!$C$76</definedName>
     <definedName name="Инвойс_упаковка">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_упаковка_п">Com_Invoice!#REF!</definedName>
     <definedName name="Инвойс_условия">Com_Invoice!$D$14</definedName>
-    <definedName name="Инвойс_условия_п">Com_Invoice!$D$73</definedName>
+    <definedName name="Инвойс_условия_п">Com_Invoice!$D$80</definedName>
     <definedName name="Инвойс_цена">Com_Invoice!$E$16</definedName>
-    <definedName name="Инвойс_цена_п">Com_Invoice!$E$75</definedName>
+    <definedName name="Инвойс_цена_п">Com_Invoice!$E$82</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="МСЦ">Com_Invoice!$E$4</definedName>
-    <definedName name="МСЦ_п">Com_Invoice!$E$63</definedName>
+    <definedName name="МСЦ_п">Com_Invoice!$E$70</definedName>
     <definedName name="МСЦ_сертификат">Com_Invoice!$F$4</definedName>
-    <definedName name="МСЦ_сертификат_п">Com_Invoice!$F$63</definedName>
+    <definedName name="МСЦ_сертификат_п">Com_Invoice!$F$70</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
     <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
@@ -122,10 +123,6 @@
     <definedName name="Продавец_заголовок">Export_Contract!$A$5</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$A$9</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$A$8</definedName>
-    <definedName name="Прочие_условия_заголовок">Export_Contract!$A$28</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$A$29</definedName>
-    <definedName name="Сертификаты_массив">Export_Contract!$A$27</definedName>
-    <definedName name="Сертификаты_описание">Export_Contract!$A$26</definedName>
     <definedName name="Соглашение">Export_Contract!$A$1</definedName>
     <definedName name="Стороны_заголовок">Export_Contract!$A$4</definedName>
     <definedName name="Цена_всего">Export_Contract!$A$22</definedName>
@@ -154,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="152">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -415,42 +412,6 @@
   </si>
   <si>
     <t>3. Доставка</t>
-  </si>
-  <si>
-    <t>3.1. The commodity should be delivered under terms of CFR Busan</t>
-  </si>
-  <si>
-    <t>3.1. Поставка осуществляется на условиях CFR Пусан</t>
-  </si>
-  <si>
-    <t>3.5 The delivery of goods to Buyer, mentioned in clause 1.1 of this Agreement should be carried in port of destination Busan, Korea</t>
-  </si>
-  <si>
-    <t>3.5. Передача Покупателю Товара, оговоренного в п.1.1. настоящего Дополнения будет производиться в порту назначения Пусан, Корея</t>
-  </si>
-  <si>
-    <t>Seller is oligated to issue set of certificates for following companies:</t>
-  </si>
-  <si>
-    <t>Покупатель обязуется выпустить комплект сертификатов на следующих получателей:</t>
-  </si>
-  <si>
-    <t>4  Other terms</t>
-  </si>
-  <si>
-    <t>4.  Прочие условия</t>
-  </si>
-  <si>
-    <t>Copies of present agreement corresponded by fax are also valid.</t>
-  </si>
-  <si>
-    <t>Копии настоящего дополнения, подписанные по факсу, имеют юридическую силу.</t>
-  </si>
-  <si>
-    <t>5.  Addresses of the Parties</t>
-  </si>
-  <si>
-    <t>5.  Адреса Сторон</t>
   </si>
   <si>
     <t xml:space="preserve">Продавец: </t>
@@ -584,22 +545,6 @@
     MSC Frozen Alaska Pollock Roe - 222,021 tn (net weight)</t>
   </si>
   <si>
-    <t>2) RONGCHENG KANGBAO AQUATIC FOODS CO., LTD.
-NO.189 XUNSHAN ROAD, XUNSHAN STREET, RONGCHENG, WEIHAI, SHANDONG PROVINCE	
-*  f/v "Morskoy Volk"
-    MSC Frozen Alaska Pollock Milts - 29,585 tn (net weight)
-*  f/v "Sea Hunter"
-    MSC Frozen Alaska Pollock Roe - 222,021 tn (net weight)</t>
-  </si>
-  <si>
-    <t>2) RONGCHENG KANGBAO AQUATIC FOODS CO., LTD.
-NO.189 XUNSHAN ROAD, XUNSHAN STREET, RONGCHENG, WEIHAI, SHANDONG PROVINCE	
-*  МФТ "Морской Волк"
-    MSC Молоки минтая мороженые - 29,585 тн (нетто)
-*  МФТ "Морской Волк"
-    MSC Икра минтая - 222,021 тн (нетто)</t>
-  </si>
-  <si>
     <t>СТРАНА ПРОИСХОЖДЕНИЯ РОССИЯ</t>
   </si>
   <si>
@@ -646,6 +591,32 @@
   </si>
   <si>
     <t>Подписано Котов Н.М.</t>
+  </si>
+  <si>
+    <t>4.  Addresses of the Parties</t>
+  </si>
+  <si>
+    <t>4.  Адреса Сторон</t>
+  </si>
+  <si>
+    <t>3.1 Supply of products is carried out on FCA Terms.
+Acceptance- transfer of Goods by quantity and quality is made on the territory of the Russian Federation in Zarubino.</t>
+  </si>
+  <si>
+    <t>3.1 Поставка осуществляется на условиях FCA.
+Приемка-передача Товара по количеству и качеству производится на территории Российской Федерации в п. Зарубино</t>
+  </si>
+  <si>
+    <t>3.4 The Parties have agreed that the acceptance and transfer of the batch of Goods in the settlement of Zarubino on behalf of the Buyer will be carried out by: KTI COMPANY LIMITED 7, Chungjang-daero, Jung-gu, Busan, Republic of Korea (Jungang-dong-4ga, KYOBO B/D 2,3F)</t>
+  </si>
+  <si>
+    <t>3.4 Стороны пришли к соглашению, что приемку-передачу партии Товара в п. Зарубино от имени покупателя будет осуществлять: KTI COMPANY LIMITED 7, Chungjang-daero, Jung-gu, Busan, Republic of Korea (Jungang-dong-4ga, KYOBO B/D 2,3F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected delivery date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата поставки ориентировочно </t>
   </si>
 </sst>
 </file>
@@ -656,7 +627,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="\ &quot;@* &quot;\ "/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +702,17 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -915,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1005,9 +987,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1200,9 +1179,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1241,6 +1217,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,10 +1545,10 @@
     <tabColor theme="9" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W85"/>
+  <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A27" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1593,10 +1578,10 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="G1"/>
@@ -1635,7 +1620,7 @@
     </row>
     <row r="3" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>67</v>
@@ -1658,11 +1643,11 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:22" s="98" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="99" t="s">
+    <row r="4" spans="1:22" s="97" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="99" t="s">
         <v>69</v>
       </c>
       <c r="F4" s="10"/>
@@ -1694,7 +1679,7 @@
     </row>
     <row r="6" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="21" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>48</v>
@@ -1714,7 +1699,7 @@
     </row>
     <row r="7" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>50</v>
@@ -1722,7 +1707,7 @@
     </row>
     <row r="8" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>72</v>
@@ -1730,7 +1715,7 @@
     </row>
     <row r="9" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="17" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>73</v>
@@ -1803,7 +1788,7 @@
     </row>
     <row r="13" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>76</v>
@@ -1827,10 +1812,10 @@
     </row>
     <row r="16" spans="1:22" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -1852,10 +1837,10 @@
     </row>
     <row r="17" spans="1:22" ht="35.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -1948,18 +1933,18 @@
     </row>
     <row r="21" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="25" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:22" s="11" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>113</v>
+      <c r="A22" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>101</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1987,281 +1972,257 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:22" ht="48.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="114" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="115" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="114" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="115" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="32" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="116" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="116" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+    </row>
+    <row r="27" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="18" t="s">
+    </row>
+    <row r="29" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="17" t="s">
+      <c r="B31" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" s="33" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="34"/>
-    </row>
-    <row r="27" spans="1:22" ht="124.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="102" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="102" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="32" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>48</v>
+      <c r="A32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="17" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="17" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>42</v>
+      <c r="A36" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="17" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>75</v>
+      <c r="A39" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="17" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="17" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="101"/>
-      <c r="B49" s="101"/>
+      <c r="A44" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="100"/>
+      <c r="B46" s="100"/>
+    </row>
+    <row r="47" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="100"/>
+      <c r="B47" s="100"/>
+    </row>
+    <row r="48" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="100"/>
+      <c r="B48" s="100"/>
+    </row>
+    <row r="49" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="100"/>
+      <c r="B49" s="100"/>
     </row>
     <row r="50" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="101"/>
-      <c r="B50" s="101"/>
+      <c r="A50" s="100"/>
+      <c r="B50" s="100"/>
     </row>
     <row r="51" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="101"/>
-      <c r="B51" s="101"/>
+      <c r="A51" s="100"/>
+      <c r="B51" s="100"/>
     </row>
     <row r="52" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="101"/>
-      <c r="B52" s="101"/>
+      <c r="A52" s="100"/>
+      <c r="B52" s="100"/>
     </row>
     <row r="53" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="101"/>
-      <c r="B53" s="101"/>
+      <c r="A53" s="100"/>
+      <c r="B53" s="100"/>
     </row>
     <row r="54" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="101"/>
-      <c r="B54" s="101"/>
+      <c r="A54" s="100"/>
+      <c r="B54" s="100"/>
     </row>
     <row r="55" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="101"/>
-      <c r="B55" s="101"/>
+      <c r="A55" s="100"/>
+      <c r="B55" s="100"/>
     </row>
     <row r="56" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="101"/>
-      <c r="B56" s="101"/>
-    </row>
-    <row r="57" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="101"/>
-      <c r="B57" s="101"/>
-    </row>
-    <row r="58" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="101"/>
-      <c r="B58" s="101"/>
-    </row>
-    <row r="59" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="101"/>
-      <c r="B59" s="101"/>
-    </row>
+      <c r="A56" s="100"/>
+      <c r="B56" s="100"/>
+    </row>
+    <row r="57" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="62" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="65" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="66" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="67" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="68" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="69" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="70" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="71" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{13E4E285-FA5D-41CC-AC7F-578EA8AF8279}">
@@ -2283,10 +2244,10 @@
     <tabColor theme="9" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Y106"/>
+  <dimension ref="A2:Y113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A66" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2308,206 +2269,206 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51"/>
-      <c r="B3" s="112" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="38" t="s">
+      <c r="C3" s="111"/>
+      <c r="D3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="49"/>
       <c r="P3">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="51"/>
-      <c r="B4" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="46" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="49"/>
       <c r="P4">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="51"/>
-      <c r="B5" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="50"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="42"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="49"/>
       <c r="P5">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="52" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="50"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="49"/>
       <c r="P6">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="51"/>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="55" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="50"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="43"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="51"/>
-      <c r="B8" s="107" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" s="110"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="50"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="105" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="106"/>
+      <c r="D8" s="107" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="108"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="51"/>
-      <c r="B9" s="57" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="50"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="51"/>
-      <c r="B10" s="58" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="50"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="49"/>
     </row>
     <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="55" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="50"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="49"/>
     </row>
     <row r="12" spans="1:25" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="51"/>
-      <c r="B12" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="67" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="63"/>
+      <c r="D12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="50"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="51"/>
-      <c r="B13" s="50" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="52" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="50"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="51"/>
-      <c r="B14" s="50"/>
-      <c r="D14" s="55" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="49"/>
+      <c r="D14" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="50"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:25" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="51"/>
-      <c r="B15" s="91" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="91" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="97" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="91" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="93" t="s">
+      <c r="D15" s="96" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="90" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="50"/>
+      <c r="G15" s="49"/>
       <c r="P15" t="s">
         <v>29</v>
       </c>
@@ -2540,50 +2501,50 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="51"/>
-      <c r="B16" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" s="105" t="s">
-        <v>149</v>
-      </c>
-      <c r="E16" s="70" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="103" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="50"/>
+      <c r="G16" s="49"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A17" s="51"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A18" s="51"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A19" s="51"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="49"/>
       <c r="P19" t="s">
         <v>29</v>
       </c>
@@ -2607,190 +2568,190 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A20" s="51"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="49"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A21" s="51"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A22" s="51"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="49"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A23" s="51"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="50"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A24" s="51"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="49"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A25" s="51"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="50"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A26" s="51"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A27" s="51"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="50"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A28" s="51"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="49"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A29" s="51"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="50"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A30" s="51"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="49"/>
       <c r="P30">
         <v>33547.5</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A31" s="51"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="49"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A32" s="51"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="49"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="51"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="50"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="49"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="51"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="50"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="49"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="51"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="51"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
+      <c r="A36" s="50"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="49"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="51"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="50"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="49"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="51"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="50"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="49"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="51"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="50"/>
+      <c r="G39" s="49"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="51"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
@@ -2798,667 +2759,695 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="50"/>
+      <c r="G40" s="49"/>
     </row>
     <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="51"/>
-      <c r="B41" s="73" t="s">
+      <c r="A41" s="50"/>
+      <c r="B41" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="50"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="49"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="51"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="76" t="s">
-        <v>146</v>
-      </c>
-      <c r="D42" s="106" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" s="77"/>
-      <c r="F42" s="78" t="s">
-        <v>135</v>
-      </c>
-      <c r="G42" s="50"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="104" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" s="76"/>
+      <c r="F42" s="77" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="51"/>
-      <c r="B43" s="115" t="s">
+      <c r="A43" s="50"/>
+      <c r="B43" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="50"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="49"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="51"/>
-      <c r="B44" s="79" t="s">
+      <c r="A44" s="50"/>
+      <c r="B44" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="80"/>
-      <c r="D44" s="52" t="s">
+      <c r="C44" s="79"/>
+      <c r="D44" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="53"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="50"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="49"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="51"/>
-      <c r="B45" s="46" t="s">
+      <c r="A45" s="50"/>
+      <c r="B45" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="50"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="50"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="49"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="49"/>
     </row>
     <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="51"/>
-      <c r="B46" s="46" t="s">
+      <c r="A46" s="50"/>
+      <c r="B46" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="50"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="50"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="49"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="49"/>
     </row>
     <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="51"/>
-      <c r="B47" s="46" t="s">
+      <c r="A47" s="50"/>
+      <c r="B47" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="47"/>
-      <c r="D47" s="50"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="50"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="49"/>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="51"/>
-      <c r="B48" s="67" t="s">
+      <c r="A48" s="50"/>
+      <c r="B48" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="68"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="66"/>
-      <c r="G48" s="50"/>
-    </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-    </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-    </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="44"/>
-      <c r="C53" s="44"/>
-    </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="44"/>
-      <c r="C54" s="44"/>
-    </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-    </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="44"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="44"/>
-      <c r="C60" s="44"/>
-    </row>
-    <row r="61" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="B61" s="96" t="s">
+      <c r="C48" s="67"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="49"/>
+    </row>
+    <row r="49" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+    </row>
+    <row r="50" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+    </row>
+    <row r="51" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+    </row>
+    <row r="52" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+    </row>
+    <row r="53" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+    </row>
+    <row r="54" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+    </row>
+    <row r="55" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+    </row>
+    <row r="56" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+    </row>
+    <row r="57" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+    </row>
+    <row r="58" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+    </row>
+    <row r="59" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+    </row>
+    <row r="60" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+    </row>
+    <row r="61" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+    </row>
+    <row r="62" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+    </row>
+    <row r="63" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="43"/>
+      <c r="C63" s="43"/>
+    </row>
+    <row r="64" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="43"/>
+      <c r="C64" s="43"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+    </row>
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="43"/>
+    </row>
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+    </row>
+    <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="B68" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="82"/>
-      <c r="F61" s="82"/>
-    </row>
-    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="51"/>
-      <c r="B62" s="84" t="s">
+      <c r="C68" s="81"/>
+      <c r="D68" s="81"/>
+      <c r="E68" s="81"/>
+      <c r="F68" s="81"/>
+    </row>
+    <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="50"/>
+      <c r="B69" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="C62" s="84"/>
-      <c r="D62" s="83" t="s">
+      <c r="C69" s="83"/>
+      <c r="D69" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="E62" s="85" t="s">
+      <c r="E69" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="86" t="s">
+      <c r="F69" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="50"/>
-    </row>
-    <row r="63" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="51"/>
-      <c r="B63" s="44" t="s">
+      <c r="G69" s="49"/>
+    </row>
+    <row r="70" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="50"/>
+      <c r="B70" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="46" t="s">
+      <c r="C70" s="43"/>
+      <c r="D70" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E63" s="87" t="s">
+      <c r="E70" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="72" t="s">
+      <c r="F70" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="G63" s="50"/>
-    </row>
-    <row r="64" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="51"/>
-      <c r="B64" s="68" t="s">
+      <c r="G70" s="49"/>
+    </row>
+    <row r="71" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="50"/>
+      <c r="B71" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="68"/>
-      <c r="D64" s="55"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="51"/>
-      <c r="G64" s="50"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A65" s="51"/>
-      <c r="B65" s="88" t="s">
+      <c r="C71" s="67"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="49"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72" s="50"/>
+      <c r="B72" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="C65" s="84"/>
-      <c r="D65" s="52" t="s">
+      <c r="C72" s="83"/>
+      <c r="D72" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" s="52"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="49"/>
+    </row>
+    <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="50"/>
+      <c r="B73" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="46"/>
+      <c r="D73" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73" s="43"/>
+      <c r="F73" s="55"/>
+      <c r="G73" s="49"/>
+    </row>
+    <row r="74" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="50"/>
+      <c r="B74" s="108" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="108"/>
+      <c r="D74" s="107" t="s">
+        <v>133</v>
+      </c>
+      <c r="E74" s="108"/>
+      <c r="F74" s="109"/>
+      <c r="G74" s="49"/>
+    </row>
+    <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="50"/>
+      <c r="B75" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="D75" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E75" s="52"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="49"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="50"/>
+      <c r="B76" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" s="59"/>
+      <c r="F76" s="60"/>
+      <c r="G76" s="49"/>
+    </row>
+    <row r="77" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="50"/>
+      <c r="B77" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="89"/>
+      <c r="D77" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E77" s="43"/>
+      <c r="F77" s="55"/>
+      <c r="G77" s="49"/>
+    </row>
+    <row r="78" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="50"/>
+      <c r="B78" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78" s="67"/>
+      <c r="D78" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E78" s="67"/>
+      <c r="F78" s="68"/>
+      <c r="G78" s="49"/>
+    </row>
+    <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="50"/>
+      <c r="B79" t="s">
+        <v>116</v>
+      </c>
+      <c r="D79" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E79" s="52"/>
+      <c r="F79" s="53"/>
+      <c r="G79" s="49"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A80" s="50"/>
+      <c r="D80" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="E80" s="67"/>
+      <c r="F80" s="68"/>
+      <c r="G80" s="49"/>
+    </row>
+    <row r="81" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="50"/>
+      <c r="B81" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="90" t="s">
+        <v>142</v>
+      </c>
+      <c r="D81" s="91" t="s">
+        <v>136</v>
+      </c>
+      <c r="E81" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="F81" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="G81" s="49"/>
+    </row>
+    <row r="82" spans="1:15" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="50"/>
+      <c r="B82" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82" s="69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D82" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="E82" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="F82" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G82" s="49"/>
+    </row>
+    <row r="83" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="50"/>
+      <c r="B83" s="69"/>
+      <c r="C83" s="69"/>
+      <c r="D83" s="69"/>
+      <c r="E83" s="69"/>
+      <c r="F83" s="48"/>
+      <c r="G83" s="49"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A84" s="50"/>
+      <c r="B84" s="69"/>
+      <c r="C84" s="69"/>
+      <c r="D84" s="69"/>
+      <c r="E84" s="69"/>
+      <c r="F84" s="48"/>
+      <c r="G84" s="49"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A85" s="50"/>
+      <c r="B85" s="69"/>
+      <c r="C85" s="69"/>
+      <c r="D85" s="69"/>
+      <c r="E85" s="69"/>
+      <c r="F85" s="48"/>
+      <c r="G85" s="49"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A86" s="50"/>
+      <c r="E86" s="69"/>
+      <c r="F86" s="48"/>
+      <c r="G86" s="49"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A87" s="50"/>
+      <c r="B87" s="69"/>
+      <c r="C87" s="69"/>
+      <c r="D87" s="69"/>
+      <c r="E87" s="69"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="49"/>
+      <c r="O87" s="93"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A88" s="50"/>
+      <c r="B88" s="69"/>
+      <c r="C88" s="69"/>
+      <c r="D88" s="69"/>
+      <c r="E88" s="69"/>
+      <c r="F88" s="48"/>
+      <c r="G88" s="49"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A89" s="50"/>
+      <c r="B89" s="69"/>
+      <c r="C89" s="69"/>
+      <c r="D89" s="69"/>
+      <c r="E89" s="69"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="49"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A90" s="50"/>
+      <c r="B90" s="69"/>
+      <c r="C90" s="69"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="69"/>
+      <c r="F90" s="48"/>
+      <c r="G90" s="49"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A91" s="50"/>
+      <c r="B91" s="69"/>
+      <c r="C91" s="69"/>
+      <c r="D91" s="69"/>
+      <c r="E91" s="69"/>
+      <c r="F91" s="48"/>
+      <c r="G91" s="49"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A92" s="50"/>
+      <c r="B92" s="69"/>
+      <c r="C92" s="69"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="69"/>
+      <c r="F92" s="48"/>
+      <c r="G92" s="49"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A93" s="50"/>
+      <c r="B93" s="69"/>
+      <c r="C93" s="69"/>
+      <c r="D93" s="69"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="48"/>
+      <c r="G93" s="49"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A94" s="50"/>
+      <c r="B94" s="69"/>
+      <c r="C94" s="69"/>
+      <c r="D94" s="69"/>
+      <c r="E94" s="69"/>
+      <c r="F94" s="48"/>
+      <c r="G94" s="49"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A95" s="50"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="69"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="69"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="49"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A96" s="50"/>
+      <c r="B96" s="69"/>
+      <c r="C96" s="69"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="69"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="49"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A97" s="50"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="69"/>
+      <c r="E97" s="69"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="49"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A98" s="50"/>
+      <c r="B98" s="69"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="48"/>
+      <c r="G98" s="49"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A99" s="50"/>
+      <c r="B99" s="69"/>
+      <c r="C99" s="69"/>
+      <c r="D99" s="69"/>
+      <c r="E99" s="69"/>
+      <c r="F99" s="48"/>
+      <c r="G99" s="49"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A100" s="50"/>
+      <c r="B100" s="69"/>
+      <c r="C100" s="69"/>
+      <c r="D100" s="69"/>
+      <c r="E100" s="69"/>
+      <c r="F100" s="48"/>
+      <c r="G100" s="49"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A101" s="50"/>
+      <c r="B101" s="69"/>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="48"/>
+      <c r="G101" s="49"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A102" s="50"/>
+      <c r="B102" s="69"/>
+      <c r="C102" s="69"/>
+      <c r="D102" s="69"/>
+      <c r="E102" s="69"/>
+      <c r="F102" s="48"/>
+      <c r="G102" s="49"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A103" s="50"/>
+      <c r="B103" s="44"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="61"/>
+      <c r="G103" s="49"/>
+    </row>
+    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="50"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="49"/>
+    </row>
+    <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A105" s="50"/>
+      <c r="B105" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="49"/>
+    </row>
+    <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A106" s="50"/>
+      <c r="B106" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106" s="73"/>
+      <c r="D106" s="73"/>
+      <c r="E106" s="73"/>
+      <c r="F106" s="74"/>
+      <c r="G106" s="49"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A107" s="50"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="D107" s="102" t="s">
+        <v>124</v>
+      </c>
+      <c r="E107" s="76"/>
+      <c r="F107" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="G107" s="49"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A108" s="50"/>
+      <c r="B108" s="112" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="112"/>
+      <c r="D108" s="112"/>
+      <c r="E108" s="76"/>
+      <c r="F108" s="61"/>
+      <c r="G108" s="49"/>
+    </row>
+    <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A109" s="50"/>
+      <c r="B109" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C109" s="79"/>
+      <c r="D109" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="E65" s="53"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="50"/>
-    </row>
-    <row r="66" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="51"/>
-      <c r="B66" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" s="47"/>
-      <c r="D66" s="55" t="s">
-        <v>147</v>
-      </c>
-      <c r="E66" s="44"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="50"/>
-    </row>
-    <row r="67" spans="1:15" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="51"/>
-      <c r="B67" s="110" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="110"/>
-      <c r="D67" s="109" t="s">
-        <v>147</v>
-      </c>
-      <c r="E67" s="110"/>
-      <c r="F67" s="111"/>
-      <c r="G67" s="50"/>
-    </row>
-    <row r="68" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="51"/>
-      <c r="B68" s="90" t="s">
-        <v>52</v>
-      </c>
-      <c r="C68" s="60" t="s">
-        <v>130</v>
-      </c>
-      <c r="D68" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="E68" s="53"/>
-      <c r="F68" s="54"/>
-      <c r="G68" s="50"/>
-    </row>
-    <row r="69" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="51"/>
-      <c r="B69" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="89" t="s">
-        <v>55</v>
-      </c>
-      <c r="D69" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E69" s="60"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="50"/>
-    </row>
-    <row r="70" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="51"/>
-      <c r="B70" s="90" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="90"/>
-      <c r="D70" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="E70" s="44"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="50"/>
-    </row>
-    <row r="71" spans="1:15" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="51"/>
-      <c r="B71" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="C71" s="68"/>
-      <c r="D71" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="E71" s="68"/>
-      <c r="F71" s="69"/>
-      <c r="G71" s="50"/>
-    </row>
-    <row r="72" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="51"/>
-      <c r="B72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D72" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="E72" s="53"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="50"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A73" s="51"/>
-      <c r="D73" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E73" s="68"/>
-      <c r="F73" s="69"/>
-      <c r="G73" s="50"/>
-    </row>
-    <row r="74" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="51"/>
-      <c r="B74" s="91" t="s">
-        <v>151</v>
-      </c>
-      <c r="C74" s="91" t="s">
-        <v>156</v>
-      </c>
-      <c r="D74" s="92" t="s">
-        <v>150</v>
-      </c>
-      <c r="E74" s="91" t="s">
-        <v>152</v>
-      </c>
-      <c r="F74" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="G74" s="50"/>
-    </row>
-    <row r="75" spans="1:15" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="51"/>
-      <c r="B75" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="C75" s="70" t="s">
-        <v>154</v>
-      </c>
-      <c r="D75" s="70" t="s">
-        <v>155</v>
-      </c>
-      <c r="E75" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="F75" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="G75" s="50"/>
-    </row>
-    <row r="76" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="51"/>
-      <c r="B76" s="70"/>
-      <c r="C76" s="70"/>
-      <c r="D76" s="70"/>
-      <c r="E76" s="70"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="50"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A77" s="51"/>
-      <c r="B77" s="70"/>
-      <c r="C77" s="70"/>
-      <c r="D77" s="70"/>
-      <c r="E77" s="70"/>
-      <c r="F77" s="49"/>
-      <c r="G77" s="50"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A78" s="51"/>
-      <c r="B78" s="70"/>
-      <c r="C78" s="70"/>
-      <c r="D78" s="70"/>
-      <c r="E78" s="70"/>
-      <c r="F78" s="49"/>
-      <c r="G78" s="50"/>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A79" s="51"/>
-      <c r="E79" s="70"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="50"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A80" s="51"/>
-      <c r="B80" s="70"/>
-      <c r="C80" s="70"/>
-      <c r="D80" s="70"/>
-      <c r="E80" s="70"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="50"/>
-      <c r="O80" s="94"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="51"/>
-      <c r="B81" s="70"/>
-      <c r="C81" s="70"/>
-      <c r="D81" s="70"/>
-      <c r="E81" s="70"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="50"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="51"/>
-      <c r="B82" s="70"/>
-      <c r="C82" s="70"/>
-      <c r="D82" s="70"/>
-      <c r="E82" s="70"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="50"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="51"/>
-      <c r="B83" s="70"/>
-      <c r="C83" s="70"/>
-      <c r="D83" s="70"/>
-      <c r="E83" s="70"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="50"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="51"/>
-      <c r="B84" s="70"/>
-      <c r="C84" s="70"/>
-      <c r="D84" s="70"/>
-      <c r="E84" s="70"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="50"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="51"/>
-      <c r="B85" s="70"/>
-      <c r="C85" s="70"/>
-      <c r="D85" s="70"/>
-      <c r="E85" s="70"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="50"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A86" s="51"/>
-      <c r="B86" s="70"/>
-      <c r="C86" s="70"/>
-      <c r="D86" s="70"/>
-      <c r="E86" s="70"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="50"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A87" s="51"/>
-      <c r="B87" s="70"/>
-      <c r="C87" s="70"/>
-      <c r="D87" s="70"/>
-      <c r="E87" s="70"/>
-      <c r="F87" s="49"/>
-      <c r="G87" s="50"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A88" s="51"/>
-      <c r="B88" s="70"/>
-      <c r="C88" s="70"/>
-      <c r="D88" s="70"/>
-      <c r="E88" s="70"/>
-      <c r="F88" s="49"/>
-      <c r="G88" s="50"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A89" s="51"/>
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="70"/>
-      <c r="E89" s="70"/>
-      <c r="F89" s="49"/>
-      <c r="G89" s="50"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A90" s="51"/>
-      <c r="B90" s="70"/>
-      <c r="C90" s="70"/>
-      <c r="D90" s="70"/>
-      <c r="E90" s="70"/>
-      <c r="F90" s="49"/>
-      <c r="G90" s="50"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A91" s="51"/>
-      <c r="B91" s="70"/>
-      <c r="C91" s="70"/>
-      <c r="D91" s="70"/>
-      <c r="E91" s="70"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="50"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A92" s="51"/>
-      <c r="B92" s="70"/>
-      <c r="C92" s="70"/>
-      <c r="D92" s="70"/>
-      <c r="E92" s="70"/>
-      <c r="F92" s="49"/>
-      <c r="G92" s="50"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A93" s="51"/>
-      <c r="B93" s="70"/>
-      <c r="C93" s="70"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70"/>
-      <c r="F93" s="49"/>
-      <c r="G93" s="50"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A94" s="51"/>
-      <c r="B94" s="70"/>
-      <c r="C94" s="70"/>
-      <c r="D94" s="70"/>
-      <c r="E94" s="70"/>
-      <c r="F94" s="49"/>
-      <c r="G94" s="50"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A95" s="51"/>
-      <c r="B95" s="70"/>
-      <c r="C95" s="70"/>
-      <c r="D95" s="70"/>
-      <c r="E95" s="70"/>
-      <c r="F95" s="49"/>
-      <c r="G95" s="50"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A96" s="51"/>
-      <c r="B96" s="45"/>
-      <c r="C96" s="45"/>
-      <c r="D96" s="45"/>
-      <c r="E96" s="77"/>
-      <c r="F96" s="62"/>
-      <c r="G96" s="50"/>
-    </row>
-    <row r="97" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="51"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="50"/>
-    </row>
-    <row r="98" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="51"/>
-      <c r="B98" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="50"/>
-    </row>
-    <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="51"/>
-      <c r="B99" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="C99" s="74"/>
-      <c r="D99" s="74"/>
-      <c r="E99" s="74"/>
-      <c r="F99" s="75"/>
-      <c r="G99" s="50"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A100" s="51"/>
-      <c r="B100" s="39"/>
-      <c r="C100" s="76" t="s">
-        <v>145</v>
-      </c>
-      <c r="D100" s="104" t="s">
-        <v>136</v>
-      </c>
-      <c r="E100" s="77"/>
-      <c r="F100" s="78" t="s">
-        <v>137</v>
-      </c>
-      <c r="G100" s="50"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A101" s="51"/>
-      <c r="B101" s="114" t="s">
-        <v>38</v>
-      </c>
-      <c r="C101" s="114"/>
-      <c r="D101" s="114"/>
-      <c r="E101" s="77"/>
-      <c r="F101" s="62"/>
-      <c r="G101" s="50"/>
-    </row>
-    <row r="102" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A102" s="51"/>
-      <c r="B102" s="80" t="s">
-        <v>39</v>
-      </c>
-      <c r="C102" s="80"/>
-      <c r="D102" s="52" t="s">
-        <v>157</v>
-      </c>
-      <c r="E102" s="53"/>
-      <c r="F102" s="54"/>
-      <c r="G102" s="50"/>
-    </row>
-    <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="51"/>
-      <c r="B103" s="47" t="s">
+      <c r="E109" s="52"/>
+      <c r="F109" s="53"/>
+      <c r="G109" s="49"/>
+    </row>
+    <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A110" s="50"/>
+      <c r="B110" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C103" s="47"/>
-      <c r="D103" s="50"/>
-      <c r="F103" s="51"/>
-      <c r="G103" s="50"/>
-    </row>
-    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="51"/>
-      <c r="B104" s="47" t="s">
+      <c r="C110" s="46"/>
+      <c r="D110" s="49"/>
+      <c r="F110" s="50"/>
+      <c r="G110" s="49"/>
+    </row>
+    <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A111" s="50"/>
+      <c r="B111" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C104" s="47"/>
-      <c r="D104" s="50"/>
-      <c r="F104" s="51"/>
-      <c r="G104" s="50"/>
-    </row>
-    <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="51"/>
-      <c r="B105" s="47" t="s">
+      <c r="C111" s="46"/>
+      <c r="D111" s="49"/>
+      <c r="F111" s="50"/>
+      <c r="G111" s="49"/>
+    </row>
+    <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A112" s="50"/>
+      <c r="B112" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C105" s="47"/>
-      <c r="D105" s="50"/>
-      <c r="F105" s="51"/>
-      <c r="G105" s="50"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A106" s="51"/>
-      <c r="B106" s="68" t="s">
+      <c r="C112" s="46"/>
+      <c r="D112" s="49"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="49"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A113" s="50"/>
+      <c r="B113" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="C106" s="68"/>
-      <c r="D106" s="81"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="66"/>
-      <c r="G106" s="50"/>
+      <c r="C113" s="67"/>
+      <c r="D113" s="80"/>
+      <c r="E113" s="64"/>
+      <c r="F113" s="65"/>
+      <c r="G113" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:F74"/>
     <mergeCell ref="B43:D43"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="57" max="6" man="1"/>
+    <brk id="64" max="6" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Export Route minor fix + minor fix in contract tmp date cell width
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3C2B6B-89BB-4773-9D27-84F622AD8F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB3912C-AA73-4FCF-B02E-EB0AF9FEA942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16394" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -171,9 +171,6 @@
     <t>"Tikhrybcom Co., LTD"</t>
   </si>
   <si>
-    <t>32T from March 10, 2023</t>
-  </si>
-  <si>
     <t>MSC certified</t>
   </si>
   <si>
@@ -617,6 +614,9 @@
   </si>
   <si>
     <t xml:space="preserve">Дата поставки ориентировочно </t>
+  </si>
+  <si>
+    <t>32T from December 10, 2023</t>
   </si>
 </sst>
 </file>
@@ -1191,6 +1191,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1217,15 +1226,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1547,7 +1547,7 @@
   </sheetPr>
   <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A21" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1578,10 +1578,10 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="G1"/>
@@ -1599,10 +1599,10 @@
     </row>
     <row r="2" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1"/>
       <c r="G2"/>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="3" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -1645,10 +1645,10 @@
     </row>
     <row r="4" spans="1:22" s="97" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="99" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="99" t="s">
-        <v>69</v>
       </c>
       <c r="F4" s="10"/>
       <c r="S4" s="10"/>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="5" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>71</v>
       </c>
       <c r="D5" s="1"/>
       <c r="G5"/>
@@ -1679,10 +1679,10 @@
     </row>
     <row r="6" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
@@ -1699,26 +1699,26 @@
     </row>
     <row r="7" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9"/>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="10" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -1760,10 +1760,10 @@
     </row>
     <row r="11" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -1780,42 +1780,42 @@
     </row>
     <row r="12" spans="1:22" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>112</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>113</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -1837,10 +1837,10 @@
     </row>
     <row r="17" spans="1:22" ht="35.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="19" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>81</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -1908,10 +1908,10 @@
     </row>
     <row r="20" spans="1:22" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -1933,18 +1933,18 @@
     </row>
     <row r="21" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>120</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:22" s="11" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -1966,34 +1966,34 @@
     </row>
     <row r="23" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="24" spans="1:22" ht="48.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="114" t="s">
+      <c r="A24" s="105" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="B24" s="115" t="s">
+    </row>
+    <row r="25" spans="1:22" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="105" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="114" t="s">
+      <c r="B25" s="106" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="115" t="s">
+    </row>
+    <row r="26" spans="1:22" s="32" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="107" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" s="32" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="116" t="s">
+      <c r="B26" s="107" t="s">
         <v>150</v>
-      </c>
-      <c r="B26" s="116" t="s">
-        <v>151</v>
       </c>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
@@ -2015,18 +2015,18 @@
     </row>
     <row r="27" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>144</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -2034,135 +2034,135 @@
         <v>5</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>91</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
@@ -2246,16 +2246,16 @@
   </sheetPr>
   <dimension ref="A2:Y113"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.53125" customWidth="1"/>
     <col min="2" max="2" width="15.265625" customWidth="1"/>
-    <col min="3" max="3" width="48.9296875" customWidth="1"/>
-    <col min="4" max="4" width="22.796875" customWidth="1"/>
+    <col min="3" max="3" width="46.73046875" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.796875" customWidth="1"/>
     <col min="7" max="7" width="2.3984375" customWidth="1"/>
@@ -2279,10 +2279,10 @@
     </row>
     <row r="3" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50"/>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="111"/>
+      <c r="C3" s="114"/>
       <c r="D3" s="37" t="s">
         <v>2</v>
       </c>
@@ -2300,17 +2300,17 @@
     <row r="4" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="50"/>
       <c r="B4" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="F4" s="48" t="s">
         <v>7</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>8</v>
       </c>
       <c r="G4" s="49"/>
       <c r="P4">
@@ -2320,7 +2320,7 @@
     <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="50"/>
       <c r="B5" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="101"/>
@@ -2334,11 +2334,11 @@
     <row r="6" spans="1:25" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="50"/>
       <c r="B6" s="51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="52"/>
       <c r="D6" s="51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="53"/>
@@ -2350,11 +2350,11 @@
     <row r="7" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="50"/>
       <c r="B7" s="45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="43"/>
       <c r="F7" s="55"/>
@@ -2362,27 +2362,27 @@
     </row>
     <row r="8" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="50"/>
-      <c r="B8" s="105" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="107" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="108"/>
-      <c r="F8" s="109"/>
+      <c r="B8" s="108" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="109"/>
+      <c r="D8" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="111"/>
+      <c r="F8" s="112"/>
       <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="50"/>
       <c r="B9" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="51" t="s">
         <v>17</v>
-      </c>
-      <c r="D9" s="51" t="s">
-        <v>18</v>
       </c>
       <c r="E9" s="52"/>
       <c r="F9" s="53"/>
@@ -2391,13 +2391,13 @@
     <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="50"/>
       <c r="B10" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="D10" s="37" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>21</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="60"/>
@@ -2406,11 +2406,11 @@
     <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="50"/>
       <c r="B11" s="56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="43"/>
       <c r="F11" s="55"/>
@@ -2419,11 +2419,11 @@
     <row r="12" spans="1:25" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="50"/>
       <c r="B12" s="62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="63"/>
       <c r="D12" s="66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="67"/>
       <c r="F12" s="68"/>
@@ -2432,10 +2432,10 @@
     <row r="13" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="50"/>
       <c r="B13" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="52"/>
       <c r="F13" s="53"/>
@@ -2445,7 +2445,7 @@
       <c r="A14" s="50"/>
       <c r="B14" s="49"/>
       <c r="D14" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="43"/>
       <c r="F14" s="55"/>
@@ -2454,32 +2454,32 @@
     <row r="15" spans="1:25" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="50"/>
       <c r="B15" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="90" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="96" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="92" t="s">
         <v>27</v>
-      </c>
-      <c r="D15" s="96" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="90" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="92" t="s">
-        <v>28</v>
       </c>
       <c r="G15" s="49"/>
       <c r="P15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>30</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>31</v>
-      </c>
-      <c r="S15" t="s">
-        <v>32</v>
       </c>
       <c r="T15">
         <v>426</v>
@@ -2497,25 +2497,25 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="50"/>
       <c r="B16" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="48" t="s">
         <v>34</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>35</v>
       </c>
       <c r="G16" s="49"/>
     </row>
@@ -2546,10 +2546,10 @@
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
       <c r="P19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R19">
         <v>22.500000000000004</v>
@@ -2753,7 +2753,7 @@
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="50"/>
       <c r="B40" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -2764,7 +2764,7 @@
     <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="50"/>
       <c r="B41" s="72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="73"/>
       <c r="D41" s="73"/>
@@ -2776,24 +2776,24 @@
       <c r="A42" s="50"/>
       <c r="B42" s="56"/>
       <c r="C42" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D42" s="104" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E42" s="76"/>
       <c r="F42" s="77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="50"/>
-      <c r="B43" s="113" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
+      <c r="B43" s="116" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="115"/>
+      <c r="D43" s="115"/>
       <c r="E43" s="76"/>
       <c r="F43" s="61"/>
       <c r="G43" s="49"/>
@@ -2801,11 +2801,11 @@
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="50"/>
       <c r="B44" s="78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="79"/>
       <c r="D44" s="51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E44" s="52"/>
       <c r="F44" s="53"/>
@@ -2814,7 +2814,7 @@
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="50"/>
       <c r="B45" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="46"/>
       <c r="D45" s="49"/>
@@ -2824,7 +2824,7 @@
     <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="50"/>
       <c r="B46" s="45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="46"/>
       <c r="D46" s="49"/>
@@ -2834,7 +2834,7 @@
     <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="50"/>
       <c r="B47" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="46"/>
       <c r="D47" s="49"/>
@@ -2844,7 +2844,7 @@
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="50"/>
       <c r="B48" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="67"/>
       <c r="D48" s="80"/>
@@ -2929,7 +2929,7 @@
     </row>
     <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
       <c r="B68" s="95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C68" s="81"/>
       <c r="D68" s="81"/>
@@ -2939,11 +2939,11 @@
     <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="50"/>
       <c r="B69" s="83" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C69" s="83"/>
       <c r="D69" s="82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E69" s="84" t="s">
         <v>3</v>
@@ -2956,24 +2956,24 @@
     <row r="70" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="50"/>
       <c r="B70" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" s="43"/>
       <c r="D70" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E70" s="86" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="71" t="s">
         <v>7</v>
-      </c>
-      <c r="F70" s="71" t="s">
-        <v>8</v>
       </c>
       <c r="G70" s="49"/>
     </row>
     <row r="71" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="50"/>
       <c r="B71" s="67" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C71" s="67"/>
       <c r="D71" s="54"/>
@@ -2984,11 +2984,11 @@
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="50"/>
       <c r="B72" s="87" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" s="83"/>
       <c r="D72" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E72" s="52"/>
       <c r="F72" s="53"/>
@@ -2997,11 +2997,11 @@
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="50"/>
       <c r="B73" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73" s="46"/>
       <c r="D73" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E73" s="43"/>
       <c r="F73" s="55"/>
@@ -3009,27 +3009,27 @@
     </row>
     <row r="74" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="50"/>
-      <c r="B74" s="108" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="108"/>
-      <c r="D74" s="107" t="s">
-        <v>133</v>
-      </c>
-      <c r="E74" s="108"/>
-      <c r="F74" s="109"/>
+      <c r="B74" s="111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="111"/>
+      <c r="D74" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="E74" s="111"/>
+      <c r="F74" s="112"/>
       <c r="G74" s="49"/>
     </row>
     <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="50"/>
       <c r="B75" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="51" t="s">
         <v>52</v>
-      </c>
-      <c r="C75" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" s="51" t="s">
-        <v>53</v>
       </c>
       <c r="E75" s="52"/>
       <c r="F75" s="53"/>
@@ -3038,13 +3038,13 @@
     <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="50"/>
       <c r="B76" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="C76" s="88" t="s">
+      <c r="D76" s="37" t="s">
         <v>55</v>
-      </c>
-      <c r="D76" s="37" t="s">
-        <v>56</v>
       </c>
       <c r="E76" s="59"/>
       <c r="F76" s="60"/>
@@ -3053,11 +3053,11 @@
     <row r="77" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="50"/>
       <c r="B77" s="89" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C77" s="89"/>
       <c r="D77" s="54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E77" s="43"/>
       <c r="F77" s="55"/>
@@ -3066,11 +3066,11 @@
     <row r="78" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="50"/>
       <c r="B78" s="63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C78" s="67"/>
       <c r="D78" s="66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E78" s="67"/>
       <c r="F78" s="68"/>
@@ -3079,10 +3079,10 @@
     <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="50"/>
       <c r="B79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D79" s="51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E79" s="52"/>
       <c r="F79" s="53"/>
@@ -3091,7 +3091,7 @@
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="50"/>
       <c r="D80" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E80" s="67"/>
       <c r="F80" s="68"/>
@@ -3100,38 +3100,38 @@
     <row r="81" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="50"/>
       <c r="B81" s="90" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="D81" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="E81" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="D81" s="91" t="s">
-        <v>136</v>
-      </c>
-      <c r="E81" s="90" t="s">
-        <v>138</v>
-      </c>
       <c r="F81" s="92" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G81" s="49"/>
     </row>
     <row r="82" spans="1:15" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="50"/>
       <c r="B82" s="69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C82" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="D82" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="D82" s="69" t="s">
-        <v>141</v>
-      </c>
       <c r="E82" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="F82" s="48" t="s">
         <v>63</v>
-      </c>
-      <c r="F82" s="48" t="s">
-        <v>64</v>
       </c>
       <c r="G82" s="49"/>
     </row>
@@ -3334,7 +3334,7 @@
     <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="50"/>
       <c r="B105" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -3345,7 +3345,7 @@
     <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="50"/>
       <c r="B106" s="73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C106" s="73"/>
       <c r="D106" s="73"/>
@@ -3357,24 +3357,24 @@
       <c r="A107" s="50"/>
       <c r="B107" s="38"/>
       <c r="C107" s="75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D107" s="102" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E107" s="76"/>
       <c r="F107" s="77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G107" s="49"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="50"/>
-      <c r="B108" s="112" t="s">
-        <v>38</v>
-      </c>
-      <c r="C108" s="112"/>
-      <c r="D108" s="112"/>
+      <c r="B108" s="115" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="115"/>
+      <c r="D108" s="115"/>
       <c r="E108" s="76"/>
       <c r="F108" s="61"/>
       <c r="G108" s="49"/>
@@ -3382,11 +3382,11 @@
     <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="50"/>
       <c r="B109" s="79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C109" s="79"/>
       <c r="D109" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E109" s="52"/>
       <c r="F109" s="53"/>
@@ -3395,7 +3395,7 @@
     <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="50"/>
       <c r="B110" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C110" s="46"/>
       <c r="D110" s="49"/>
@@ -3405,7 +3405,7 @@
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="50"/>
       <c r="B111" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C111" s="46"/>
       <c r="D111" s="49"/>
@@ -3415,7 +3415,7 @@
     <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="50"/>
       <c r="B112" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C112" s="46"/>
       <c r="D112" s="49"/>
@@ -3425,7 +3425,7 @@
     <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" s="50"/>
       <c r="B113" s="67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C113" s="67"/>
       <c r="D113" s="80"/>

</xml_diff>

<commit_message>
fca template updated, nonComCheckbox added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E82C4-E832-4B3C-8164-3113CA2E2958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12972379-DF8F-4915-B8D9-0291EC760639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -19,32 +19,32 @@
   <definedNames>
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
-    <definedName name="Seal_agent_end">Export_Contract!$H$51</definedName>
-    <definedName name="Seal_agent_start">Export_Contract!$G$41</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$51</definedName>
-    <definedName name="Seal_seller_start">Export_Contract!$C$43</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$51</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$49</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$49</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$B$33</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$34</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$35</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$50</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$B$39</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$40</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$42</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$45</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$44</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$46</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$47</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$48</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$36</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$B$37</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$B$31</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$32</definedName>
-    <definedName name="Доставка_дата">Export_Contract!$B$26</definedName>
-    <definedName name="Доставка_приемка">Export_Contract!$B$25</definedName>
-    <definedName name="Доставка_условия">Export_Contract!$B$24</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$52</definedName>
+    <definedName name="Seal_agent_start">Export_Contract!$G$42</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$52</definedName>
+    <definedName name="Seal_seller_start">Export_Contract!$C$44</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$52</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$50</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$50</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$B$34</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$35</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$36</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$51</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$B$40</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$41</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$43</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$46</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$45</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$47</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$48</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$49</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$37</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$B$38</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$B$32</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$33</definedName>
+    <definedName name="Доставка_дата">Export_Contract!$B$27</definedName>
+    <definedName name="Доставка_приемка">Export_Contract!$B$26</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$B$25</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
     <definedName name="Инвойс_Bl_массив">Invoice!$B$21</definedName>
     <definedName name="Инвойс_банк_получателя">Invoice!$B$36</definedName>
@@ -78,9 +78,10 @@
     <definedName name="Продавец_адрес">Export_Contract!$B$8</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$B$10</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$B$9</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$B$28</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$B$29</definedName>
     <definedName name="Соглашение">Export_Contract!$B$2</definedName>
-    <definedName name="Цена_всего">Export_Contract!$B$22</definedName>
+    <definedName name="Цена_всего">Export_Contract!$B$23</definedName>
+    <definedName name="Цена_неком">Export_Contract!$B$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -103,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
   <si>
     <t>Supplementary Agreement No. 146 dated March 10, 2023</t>
   </si>
@@ -807,7 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1219,6 +1220,75 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1246,15 +1316,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1264,68 +1325,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1690,10 +1694,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF87"/>
+  <dimension ref="B1:AF88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:D27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1738,18 +1742,18 @@
       </c>
     </row>
     <row r="2" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="153" t="s">
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
       <c r="J2" s="9"/>
       <c r="L2" s="11"/>
       <c r="O2" s="10"/>
@@ -1766,18 +1770,18 @@
       <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="156" t="s">
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="179" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1794,18 +1798,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="156" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="157"/>
-      <c r="H4" s="157"/>
-      <c r="I4" s="157"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1826,18 +1830,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="159" t="s">
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1846,18 +1850,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="157" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="162" t="s">
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="157" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1902,12 +1906,12 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="165" t="s">
+      <c r="B8" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="167"/>
+      <c r="C8" s="186"/>
+      <c r="D8" s="186"/>
+      <c r="E8" s="187"/>
       <c r="F8" s="150" t="s">
         <v>10</v>
       </c>
@@ -1960,18 +1964,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="162" t="s">
+      <c r="B11" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="163"/>
-      <c r="D11" s="163"/>
-      <c r="E11" s="164"/>
-      <c r="F11" s="162" t="s">
+      <c r="C11" s="158"/>
+      <c r="D11" s="158"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="163"/>
-      <c r="H11" s="163"/>
-      <c r="I11" s="163"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="158"/>
+      <c r="I11" s="158"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2101,18 +2105,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="170" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="169"/>
-      <c r="D16" s="169"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="168" t="s">
+      <c r="F16" s="170" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="169"/>
-      <c r="H16" s="169"/>
-      <c r="I16" s="170"/>
+      <c r="G16" s="171"/>
+      <c r="H16" s="171"/>
+      <c r="I16" s="172"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2133,15 +2137,15 @@
       <c r="B17" s="150" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="171"/>
-      <c r="E17" s="172"/>
-      <c r="F17" s="173" t="s">
+      <c r="C17" s="173"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="174"/>
+      <c r="F17" s="175" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="171"/>
-      <c r="H17" s="171"/>
-      <c r="I17" s="171"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2159,16 +2163,16 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="174" t="s">
+      <c r="B18" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="175"/>
-      <c r="D18" s="175"/>
-      <c r="E18" s="175"/>
-      <c r="F18" s="174" t="s">
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="175"/>
+      <c r="G18" s="164"/>
       <c r="H18" s="23" t="s">
         <v>77</v>
       </c>
@@ -2192,16 +2196,16 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="179" t="s">
+      <c r="B19" s="168" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="180"/>
-      <c r="D19" s="180"/>
-      <c r="E19" s="180"/>
-      <c r="F19" s="179" t="s">
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="180"/>
+      <c r="G19" s="169"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2287,66 +2291,64 @@
       <c r="AC21" s="10"/>
       <c r="AD21" s="10"/>
     </row>
-    <row r="22" spans="2:30" s="30" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="2:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="189" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="189"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+    </row>
+    <row r="23" spans="2:30" s="30" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="19" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="19"/>
-    </row>
-    <row r="23" spans="2:30" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="6" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="2:30" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="6" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="22"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-      <c r="AB23" s="10"/>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10"/>
-    </row>
-    <row r="24" spans="2:30" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="176" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="177"/>
-      <c r="D24" s="177"/>
-      <c r="E24" s="178"/>
-      <c r="F24" s="176" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="177"/>
-      <c r="H24" s="177"/>
-      <c r="I24" s="177"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
       <c r="J24" s="22"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -2366,169 +2368,186 @@
       <c r="AC24" s="10"/>
       <c r="AD24" s="10"/>
     </row>
-    <row r="25" spans="2:30" s="30" customFormat="1" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="150" t="s">
+    <row r="25" spans="2:30" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="165" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="166"/>
+      <c r="D25" s="166"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="165" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="166"/>
+      <c r="H25" s="166"/>
+      <c r="I25" s="166"/>
+      <c r="J25" s="22"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+      <c r="AD25" s="10"/>
+    </row>
+    <row r="26" spans="2:30" s="30" customFormat="1" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="151"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="152"/>
-      <c r="F25" s="150" t="s">
+      <c r="C26" s="151"/>
+      <c r="D26" s="151"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="151"/>
-      <c r="H25" s="151"/>
-      <c r="I25" s="151"/>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="2:30" s="30" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="181" t="s">
+      <c r="G26" s="151"/>
+      <c r="H26" s="151"/>
+      <c r="I26" s="151"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="2:30" s="30" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="160" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="182"/>
-      <c r="D26" s="182"/>
-      <c r="E26" s="183"/>
-      <c r="F26" s="68" t="s">
+      <c r="C27" s="161"/>
+      <c r="D27" s="161"/>
+      <c r="E27" s="162"/>
+      <c r="F27" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="162" t="s">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="163"/>
-      <c r="D27" s="163"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="162" t="s">
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="163"/>
-      <c r="H27" s="163"/>
-      <c r="I27" s="164"/>
-      <c r="J27" s="22"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-      <c r="Z27" s="10"/>
-      <c r="AA27" s="10"/>
-      <c r="AB27" s="10"/>
-      <c r="AC27" s="10"/>
-      <c r="AD27" s="10"/>
-    </row>
-    <row r="28" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="150" t="s">
+      <c r="G28" s="158"/>
+      <c r="H28" s="158"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="22"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="10"/>
+      <c r="AD28" s="10"/>
+    </row>
+    <row r="29" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="151"/>
-      <c r="D28" s="151"/>
-      <c r="E28" s="152"/>
-      <c r="F28" s="150" t="s">
+      <c r="C29" s="151"/>
+      <c r="D29" s="151"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="150" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="151"/>
-      <c r="H28" s="151"/>
-      <c r="I28" s="151"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="2:30" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="162" t="s">
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="2:30" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="163"/>
-      <c r="D29" s="163"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="162" t="s">
+      <c r="C30" s="158"/>
+      <c r="D30" s="158"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="163"/>
-      <c r="H29" s="163"/>
-      <c r="I29" s="164"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="50" t="s">
+      <c r="G30" s="158"/>
+      <c r="H30" s="158"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="50" t="s">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="184" t="s">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="153" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="185"/>
-      <c r="D31" s="185"/>
-      <c r="E31" s="186"/>
-      <c r="F31" s="184" t="s">
+      <c r="C32" s="154"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="155"/>
+      <c r="F32" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="185"/>
-      <c r="H31" s="185"/>
-      <c r="I31" s="185"/>
-      <c r="J31" s="34"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="36"/>
-      <c r="AA31" s="36"/>
-      <c r="AB31" s="36"/>
-      <c r="AC31" s="36"/>
-      <c r="AD31" s="36"/>
-    </row>
-    <row r="32" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="150" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="151"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="150" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="151"/>
-      <c r="H32" s="151"/>
-      <c r="I32" s="151"/>
-      <c r="J32" s="19"/>
+      <c r="G32" s="154"/>
+      <c r="H32" s="154"/>
+      <c r="I32" s="154"/>
+      <c r="J32" s="34"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
+      <c r="AA32" s="36"/>
+      <c r="AB32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="150" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="151"/>
       <c r="D33" s="151"/>
       <c r="E33" s="152"/>
       <c r="F33" s="150" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="G33" s="151"/>
       <c r="H33" s="151"/>
@@ -2537,13 +2556,13 @@
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="150" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" s="151"/>
       <c r="D34" s="151"/>
       <c r="E34" s="152"/>
       <c r="F34" s="150" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G34" s="151"/>
       <c r="H34" s="151"/>
@@ -2552,13 +2571,13 @@
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="150" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" s="151"/>
       <c r="D35" s="151"/>
       <c r="E35" s="152"/>
       <c r="F35" s="150" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" s="151"/>
       <c r="H35" s="151"/>
@@ -2567,13 +2586,13 @@
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="150" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="151"/>
       <c r="D36" s="151"/>
       <c r="E36" s="152"/>
       <c r="F36" s="150" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G36" s="151"/>
       <c r="H36" s="151"/>
@@ -2582,13 +2601,13 @@
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="150" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37" s="151"/>
       <c r="D37" s="151"/>
       <c r="E37" s="152"/>
       <c r="F37" s="150" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G37" s="151"/>
       <c r="H37" s="151"/>
@@ -2596,162 +2615,162 @@
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="67" t="s">
+      <c r="B38" s="150" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="151"/>
+      <c r="D38" s="151"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="150" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="151"/>
+      <c r="H38" s="151"/>
+      <c r="I38" s="151"/>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="67" t="s">
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="184" t="s">
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="185"/>
-      <c r="D39" s="185"/>
-      <c r="E39" s="186"/>
-      <c r="F39" s="184" t="s">
+      <c r="C40" s="154"/>
+      <c r="D40" s="154"/>
+      <c r="E40" s="155"/>
+      <c r="F40" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="187"/>
-      <c r="H39" s="187"/>
-      <c r="I39" s="187"/>
-      <c r="J39" s="34"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
-      <c r="AA39" s="36"/>
-      <c r="AB39" s="36"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-    </row>
-    <row r="40" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="150" t="s">
+      <c r="G40" s="156"/>
+      <c r="H40" s="156"/>
+      <c r="I40" s="156"/>
+      <c r="J40" s="34"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="36"/>
+      <c r="T40" s="36"/>
+      <c r="U40" s="36"/>
+      <c r="V40" s="36"/>
+      <c r="W40" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="36"/>
+      <c r="AA40" s="36"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+    </row>
+    <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="151"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="152"/>
-      <c r="F40" s="150" t="s">
+      <c r="C41" s="151"/>
+      <c r="D41" s="151"/>
+      <c r="E41" s="152"/>
+      <c r="F41" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="151"/>
-      <c r="H40" s="151"/>
-      <c r="I40" s="151"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="19"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="151"/>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="19"/>
+    </row>
+    <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="19"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="27" t="s">
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="19"/>
+    </row>
+    <row r="43" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="27" t="s">
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="39"/>
-      <c r="C43" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="27"/>
       <c r="G43" s="28"/>
       <c r="H43" s="38"/>
       <c r="I43" s="38"/>
       <c r="J43" s="19"/>
     </row>
-    <row r="44" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G44" s="38"/>
+    <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="39"/>
+      <c r="C44" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="31"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="28"/>
       <c r="H44" s="38"/>
       <c r="I44" s="38"/>
       <c r="J44" s="19"/>
     </row>
-    <row r="45" spans="2:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="150" t="s">
+    <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="2:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="151"/>
-      <c r="D45" s="151"/>
-      <c r="E45" s="152"/>
-      <c r="F45" s="150" t="s">
+      <c r="C46" s="151"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="152"/>
+      <c r="F46" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="G45" s="151"/>
-      <c r="H45" s="151"/>
-      <c r="I45" s="152"/>
-      <c r="J45" s="19"/>
-    </row>
-    <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
+      <c r="G46" s="151"/>
+      <c r="H46" s="151"/>
+      <c r="I46" s="152"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
       <c r="F47" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
@@ -2760,78 +2779,82 @@
     </row>
     <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
       <c r="E48" s="29"/>
       <c r="F48" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="19"/>
+    </row>
+    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="19"/>
-      <c r="C49" s="36" t="s">
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="19"/>
+    </row>
+    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="19"/>
+      <c r="C50" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="12" t="s">
+      <c r="D50" s="31"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="19"/>
-    </row>
-    <row r="50" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="40" t="s">
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="19"/>
+    </row>
+    <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="41" t="s">
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="15"/>
-    </row>
-    <row r="51" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="43"/>
-      <c r="C51" s="44" t="s">
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="15"/>
+    </row>
+    <row r="52" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="43"/>
+      <c r="C52" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="45"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="44" t="s">
+      <c r="D52" s="45"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="H51" s="44" t="s">
+      <c r="H52" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="46"/>
-      <c r="J51" s="15"/>
-    </row>
-    <row r="52" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="15"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
+      <c r="I52" s="46"/>
       <c r="J52" s="15"/>
     </row>
-    <row r="53" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="15"/>
       <c r="C53" s="48"/>
       <c r="D53" s="48"/>
@@ -2930,67 +2953,33 @@
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
     </row>
-    <row r="62" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="15"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+    </row>
     <row r="63" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="80" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+    </row>
+    <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="F46:I46"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B3:E3"/>
@@ -3005,8 +2994,53 @@
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
-  <conditionalFormatting sqref="F19 J19 B20:E20 I20:J21 B21 E21">
+  <conditionalFormatting sqref="F19 J19 B20:E20 I20:J22 B21:B22 E21:E22">
     <cfRule type="notContainsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B19))&gt;0</formula>
     </cfRule>
@@ -3043,8 +3077,8 @@
   </sheetPr>
   <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
fca templates refactored, deleterows feature in setcells implemented beta
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12972379-DF8F-4915-B8D9-0291EC760639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03124B46-F32F-4024-8422-C0991F048A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -46,23 +46,24 @@
     <definedName name="Доставка_приемка">Export_Contract!$B$26</definedName>
     <definedName name="Доставка_условия">Export_Contract!$B$25</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
-    <definedName name="Инвойс_Bl_массив">Invoice!$B$21</definedName>
-    <definedName name="Инвойс_банк_получателя">Invoice!$B$36</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес">Invoice!$B$37</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт">Invoice!$B$38</definedName>
+    <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
+    <definedName name="Инвойс_банк_получателя">Invoice!$B$38</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Invoice!$B$39</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Invoice!$B$40</definedName>
     <definedName name="Инвойс_дата">Invoice!$B$5</definedName>
     <definedName name="Инвойс_дата_отправки">Invoice!#REF!</definedName>
+    <definedName name="Инвойс_декларация">Invoice!$B$20</definedName>
     <definedName name="Инвойс_изготовитель">Invoice!$B$16</definedName>
     <definedName name="Инвойс_контракт">Invoice!$B$4</definedName>
     <definedName name="Инвойс_куда">Invoice!$B$18</definedName>
     <definedName name="Инвойс_МСЦ">Invoice!$D$16</definedName>
-    <definedName name="Инвойс_подписант">Invoice!$I$36</definedName>
+    <definedName name="Инвойс_подписант">Invoice!$I$38</definedName>
     <definedName name="Инвойс_покупатель">Invoice!$B$10</definedName>
     <definedName name="Инвойс_покупатель_адрес">Invoice!$B$11</definedName>
     <definedName name="Инвойс_получатель">Invoice!$B$13</definedName>
     <definedName name="Инвойс_получатель_адрес">Invoice!$B$14</definedName>
-    <definedName name="Инвойс_получатель_в_пользу">Invoice!$B$39</definedName>
-    <definedName name="Инвойс_получатель_счет">Invoice!$B$40</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Invoice!$B$41</definedName>
+    <definedName name="Инвойс_получатель_счет">Invoice!$B$42</definedName>
     <definedName name="Инвойс_продавец">Invoice!$B$7</definedName>
     <definedName name="Инвойс_продавец_адрес">Invoice!$B$8</definedName>
     <definedName name="Инвойс_соглашение">Invoice!$B$3</definedName>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
   <si>
     <t>Supplementary Agreement No. 146 dated March 10, 2023</t>
   </si>
@@ -492,6 +493,12 @@
   </si>
   <si>
     <t>Pusan, Korea</t>
+  </si>
+  <si>
+    <t>Temporary Customs Declaration:</t>
+  </si>
+  <si>
+    <t>№ временной декларации на товары:</t>
   </si>
 </sst>
 </file>
@@ -1097,9 +1104,7 @@
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1211,6 +1216,22 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1256,15 +1277,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1327,9 +1339,6 @@
     </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1696,8 +1705,8 @@
   </sheetPr>
   <dimension ref="B1:AF88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1742,18 +1751,18 @@
       </c>
     </row>
     <row r="2" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="176" t="s">
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="177"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
       <c r="J2" s="9"/>
       <c r="L2" s="11"/>
       <c r="O2" s="10"/>
@@ -1770,18 +1779,18 @@
       <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="180" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="179" t="s">
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="180" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1798,18 +1807,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="180" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="180"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="179" t="s">
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1830,18 +1839,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="182" t="s">
+      <c r="B5" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="183"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="182" t="s">
+      <c r="C5" s="184"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="185"/>
+      <c r="F5" s="183" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="183"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
+      <c r="G5" s="184"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1850,18 +1859,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="157" t="s">
+      <c r="B6" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="157" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="161" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="158"/>
-      <c r="H6" s="158"/>
-      <c r="I6" s="158"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="162"/>
+      <c r="I6" s="162"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1906,44 +1915,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="185" t="s">
+      <c r="B8" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="187"/>
-      <c r="F8" s="150" t="s">
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="188"/>
+      <c r="F8" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="151"/>
-      <c r="H8" s="151"/>
-      <c r="I8" s="151"/>
+      <c r="G8" s="155"/>
+      <c r="H8" s="155"/>
+      <c r="I8" s="155"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="150" t="s">
+      <c r="B9" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="151"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="152"/>
-      <c r="F9" s="150" t="s">
+      <c r="C9" s="155"/>
+      <c r="D9" s="155"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="151"/>
-      <c r="H9" s="151"/>
-      <c r="I9" s="152"/>
+      <c r="G9" s="155"/>
+      <c r="H9" s="155"/>
+      <c r="I9" s="156"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="150"/>
-      <c r="C10" s="151"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="152"/>
-      <c r="F10" s="150"/>
-      <c r="G10" s="151"/>
-      <c r="H10" s="151"/>
-      <c r="I10" s="152"/>
+      <c r="B10" s="154"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="155"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="155"/>
+      <c r="H10" s="155"/>
+      <c r="I10" s="156"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -1964,18 +1973,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="157" t="s">
+      <c r="B11" s="161" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="158"/>
-      <c r="D11" s="158"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="157" t="s">
+      <c r="C11" s="162"/>
+      <c r="D11" s="162"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="161" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="158"/>
-      <c r="H11" s="158"/>
-      <c r="I11" s="158"/>
+      <c r="G11" s="162"/>
+      <c r="H11" s="162"/>
+      <c r="I11" s="162"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2018,18 +2027,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="150" t="s">
+      <c r="B13" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="151"/>
-      <c r="D13" s="151"/>
-      <c r="E13" s="152"/>
-      <c r="F13" s="150" t="s">
+      <c r="C13" s="155"/>
+      <c r="D13" s="155"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="151"/>
-      <c r="H13" s="151"/>
-      <c r="I13" s="151"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="155"/>
+      <c r="I13" s="155"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2047,18 +2056,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="151"/>
-      <c r="D14" s="151"/>
-      <c r="E14" s="152"/>
-      <c r="F14" s="150" t="s">
+      <c r="C14" s="155"/>
+      <c r="D14" s="155"/>
+      <c r="E14" s="156"/>
+      <c r="F14" s="154" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="151"/>
-      <c r="H14" s="151"/>
-      <c r="I14" s="151"/>
+      <c r="G14" s="155"/>
+      <c r="H14" s="155"/>
+      <c r="I14" s="155"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2076,18 +2085,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="151"/>
-      <c r="D15" s="151"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="150" t="s">
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="151"/>
+      <c r="G15" s="155"/>
+      <c r="H15" s="155"/>
+      <c r="I15" s="155"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2105,18 +2114,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="171" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
+      <c r="C16" s="172"/>
+      <c r="D16" s="172"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="170" t="s">
+      <c r="F16" s="171" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="171"/>
-      <c r="H16" s="171"/>
-      <c r="I16" s="172"/>
+      <c r="G16" s="172"/>
+      <c r="H16" s="172"/>
+      <c r="I16" s="173"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2134,18 +2143,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="173"/>
-      <c r="D17" s="173"/>
-      <c r="E17" s="174"/>
-      <c r="F17" s="175" t="s">
+      <c r="C17" s="174"/>
+      <c r="D17" s="174"/>
+      <c r="E17" s="175"/>
+      <c r="F17" s="176" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
+      <c r="G17" s="174"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="174"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2163,16 +2172,16 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="167" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="163" t="s">
+      <c r="C18" s="168"/>
+      <c r="D18" s="168"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="167" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="164"/>
+      <c r="G18" s="168"/>
       <c r="H18" s="23" t="s">
         <v>77</v>
       </c>
@@ -2196,16 +2205,16 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="168" t="s">
+      <c r="B19" s="169" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="169"/>
-      <c r="D19" s="169"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="168" t="s">
+      <c r="C19" s="170"/>
+      <c r="D19" s="170"/>
+      <c r="E19" s="170"/>
+      <c r="F19" s="169" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="169"/>
+      <c r="G19" s="170"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2291,14 +2300,14 @@
       <c r="AC21" s="10"/>
       <c r="AD21" s="10"/>
     </row>
-    <row r="22" spans="2:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="189" t="s">
+    <row r="22" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="148" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="189"/>
+      <c r="F22" s="148"/>
       <c r="G22" s="8"/>
       <c r="H22" s="26"/>
       <c r="I22" s="5"/>
@@ -2369,18 +2378,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="154" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="166"/>
-      <c r="D25" s="166"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="165" t="s">
+      <c r="C25" s="155"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="154" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="166"/>
-      <c r="H25" s="166"/>
-      <c r="I25" s="166"/>
+      <c r="G25" s="155"/>
+      <c r="H25" s="155"/>
+      <c r="I25" s="155"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2401,27 +2410,27 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="150" t="s">
+      <c r="B26" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="151"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="150" t="s">
+      <c r="C26" s="155"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="151"/>
-      <c r="H26" s="151"/>
-      <c r="I26" s="151"/>
+      <c r="G26" s="155"/>
+      <c r="H26" s="155"/>
+      <c r="I26" s="155"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="160" t="s">
+      <c r="B27" s="164" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="161"/>
-      <c r="D27" s="161"/>
-      <c r="E27" s="162"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="166"/>
       <c r="F27" s="68" t="s">
         <v>73</v>
       </c>
@@ -2431,18 +2440,18 @@
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="157" t="s">
+      <c r="B28" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
+      <c r="C28" s="162"/>
+      <c r="D28" s="162"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="157" t="s">
+      <c r="F28" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="158"/>
-      <c r="H28" s="158"/>
-      <c r="I28" s="159"/>
+      <c r="G28" s="162"/>
+      <c r="H28" s="162"/>
+      <c r="I28" s="163"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2463,33 +2472,33 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="150" t="s">
+      <c r="B29" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="151"/>
-      <c r="D29" s="151"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="150" t="s">
+      <c r="C29" s="155"/>
+      <c r="D29" s="155"/>
+      <c r="E29" s="156"/>
+      <c r="F29" s="154" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
+      <c r="G29" s="155"/>
+      <c r="H29" s="155"/>
+      <c r="I29" s="155"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="157" t="s">
+      <c r="B30" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="158"/>
-      <c r="D30" s="158"/>
+      <c r="C30" s="162"/>
+      <c r="D30" s="162"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="157" t="s">
+      <c r="F30" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="159"/>
+      <c r="G30" s="162"/>
+      <c r="H30" s="162"/>
+      <c r="I30" s="163"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2508,18 +2517,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="157" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="154"/>
-      <c r="D32" s="154"/>
-      <c r="E32" s="155"/>
-      <c r="F32" s="153" t="s">
+      <c r="C32" s="158"/>
+      <c r="D32" s="158"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="157" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="154"/>
-      <c r="H32" s="154"/>
-      <c r="I32" s="154"/>
+      <c r="G32" s="158"/>
+      <c r="H32" s="158"/>
+      <c r="I32" s="158"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2540,93 +2549,93 @@
       <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="150" t="s">
+      <c r="B33" s="154" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="151"/>
-      <c r="D33" s="151"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="150" t="s">
+      <c r="C33" s="155"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="151"/>
-      <c r="H33" s="151"/>
-      <c r="I33" s="151"/>
+      <c r="G33" s="155"/>
+      <c r="H33" s="155"/>
+      <c r="I33" s="155"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="150" t="s">
+      <c r="B34" s="154" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="151"/>
-      <c r="D34" s="151"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="150" t="s">
+      <c r="C34" s="155"/>
+      <c r="D34" s="155"/>
+      <c r="E34" s="156"/>
+      <c r="F34" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="151"/>
-      <c r="H34" s="151"/>
-      <c r="I34" s="151"/>
+      <c r="G34" s="155"/>
+      <c r="H34" s="155"/>
+      <c r="I34" s="155"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="150" t="s">
+      <c r="B35" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="151"/>
-      <c r="D35" s="151"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="150" t="s">
+      <c r="C35" s="155"/>
+      <c r="D35" s="155"/>
+      <c r="E35" s="156"/>
+      <c r="F35" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="151"/>
-      <c r="H35" s="151"/>
-      <c r="I35" s="151"/>
+      <c r="G35" s="155"/>
+      <c r="H35" s="155"/>
+      <c r="I35" s="155"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="150" t="s">
+      <c r="B36" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="151"/>
-      <c r="D36" s="151"/>
-      <c r="E36" s="152"/>
-      <c r="F36" s="150" t="s">
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="G36" s="151"/>
-      <c r="H36" s="151"/>
-      <c r="I36" s="151"/>
+      <c r="G36" s="155"/>
+      <c r="H36" s="155"/>
+      <c r="I36" s="155"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="150" t="s">
+      <c r="B37" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="151"/>
-      <c r="D37" s="151"/>
-      <c r="E37" s="152"/>
-      <c r="F37" s="150" t="s">
+      <c r="C37" s="155"/>
+      <c r="D37" s="155"/>
+      <c r="E37" s="156"/>
+      <c r="F37" s="154" t="s">
         <v>42</v>
       </c>
-      <c r="G37" s="151"/>
-      <c r="H37" s="151"/>
-      <c r="I37" s="151"/>
+      <c r="G37" s="155"/>
+      <c r="H37" s="155"/>
+      <c r="I37" s="155"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="150" t="s">
+      <c r="B38" s="154" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="151"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="150" t="s">
+      <c r="C38" s="155"/>
+      <c r="D38" s="155"/>
+      <c r="E38" s="156"/>
+      <c r="F38" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="G38" s="151"/>
-      <c r="H38" s="151"/>
-      <c r="I38" s="151"/>
+      <c r="G38" s="155"/>
+      <c r="H38" s="155"/>
+      <c r="I38" s="155"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2645,18 +2654,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="153" t="s">
+      <c r="B40" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="154"/>
-      <c r="D40" s="154"/>
-      <c r="E40" s="155"/>
-      <c r="F40" s="153" t="s">
+      <c r="C40" s="158"/>
+      <c r="D40" s="158"/>
+      <c r="E40" s="159"/>
+      <c r="F40" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="156"/>
-      <c r="H40" s="156"/>
-      <c r="I40" s="156"/>
+      <c r="G40" s="160"/>
+      <c r="H40" s="160"/>
+      <c r="I40" s="160"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2677,18 +2686,18 @@
       <c r="AD40" s="36"/>
     </row>
     <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="150" t="s">
+      <c r="B41" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="151"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="152"/>
-      <c r="F41" s="150" t="s">
+      <c r="C41" s="155"/>
+      <c r="D41" s="155"/>
+      <c r="E41" s="156"/>
+      <c r="F41" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="151"/>
-      <c r="H41" s="151"/>
-      <c r="I41" s="151"/>
+      <c r="G41" s="155"/>
+      <c r="H41" s="155"/>
+      <c r="I41" s="155"/>
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2748,18 +2757,18 @@
       <c r="J45" s="19"/>
     </row>
     <row r="46" spans="2:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="150" t="s">
+      <c r="B46" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="151"/>
-      <c r="D46" s="151"/>
-      <c r="E46" s="152"/>
-      <c r="F46" s="150" t="s">
+      <c r="C46" s="155"/>
+      <c r="D46" s="155"/>
+      <c r="E46" s="156"/>
+      <c r="F46" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="G46" s="151"/>
-      <c r="H46" s="151"/>
-      <c r="I46" s="152"/>
+      <c r="G46" s="155"/>
+      <c r="H46" s="155"/>
+      <c r="I46" s="156"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3075,10 +3084,10 @@
     <tabColor theme="8" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC50"/>
+  <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3425,26 +3434,26 @@
     </row>
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="57"/>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="149" t="s">
         <v>102</v>
       </c>
       <c r="C17" s="91"/>
       <c r="D17" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="92" t="s">
+      <c r="E17" s="91"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="150" t="s">
         <v>103</v>
       </c>
       <c r="I17" s="83"/>
-      <c r="J17" s="110" t="s">
+      <c r="J17" s="151" t="s">
         <v>106</v>
       </c>
-      <c r="K17" s="83"/>
-      <c r="L17" s="111"/>
-      <c r="M17" s="112"/>
+      <c r="K17" s="151"/>
+      <c r="L17" s="109"/>
+      <c r="M17" s="110"/>
       <c r="N17" s="59"/>
     </row>
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -3453,17 +3462,17 @@
         <v>123</v>
       </c>
       <c r="C18" s="88"/>
-      <c r="D18" s="113" t="s">
+      <c r="D18" s="111" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="106"/>
-      <c r="F18" s="114"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="104"/>
-      <c r="H18" s="105" t="s">
+      <c r="H18" s="153" t="s">
         <v>104</v>
       </c>
       <c r="I18" s="106"/>
-      <c r="J18" s="113" t="s">
+      <c r="J18" s="111" t="s">
         <v>56</v>
       </c>
       <c r="K18" s="106"/>
@@ -3471,411 +3480,449 @@
       <c r="M18" s="107"/>
       <c r="N18" s="59"/>
     </row>
-    <row r="19" spans="1:29" s="122" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="115"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="119"/>
-      <c r="J19" s="119"/>
-      <c r="K19" s="119"/>
-      <c r="L19" s="119"/>
-      <c r="M19" s="120"/>
-      <c r="N19" s="121"/>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-      <c r="Y19"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
-      <c r="AB19"/>
-      <c r="AC19"/>
-    </row>
-    <row r="20" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="57"/>
+      <c r="B19" s="151" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="88"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" s="106"/>
+      <c r="J19" s="111"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="107"/>
+      <c r="N19" s="59"/>
+    </row>
+    <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="57"/>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="152" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="88"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="106"/>
+      <c r="J20" s="111"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="59"/>
+    </row>
+    <row r="21" spans="1:29" s="120" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="113"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="116"/>
+      <c r="I21" s="117"/>
+      <c r="J21" s="117"/>
+      <c r="K21" s="117"/>
+      <c r="L21" s="117"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="119"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+    </row>
+    <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="57"/>
+      <c r="B22" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C22" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="63" t="s">
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="I20" s="64" t="s">
+      <c r="I22" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64" t="s">
+      <c r="J22" s="64"/>
+      <c r="K22" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="L20" s="64"/>
-      <c r="M20" s="63" t="s">
+      <c r="L22" s="64"/>
+      <c r="M22" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="N20" s="59"/>
-    </row>
-    <row r="21" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="57"/>
-      <c r="B21" s="123" t="s">
+      <c r="N22" s="59"/>
+    </row>
+    <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="57"/>
+      <c r="B23" s="121" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="149" t="s">
+      <c r="C23" s="147" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="149"/>
-      <c r="G21" s="124"/>
-      <c r="H21" s="125" t="s">
+      <c r="D23" s="147"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="147"/>
+      <c r="G23" s="122"/>
+      <c r="H23" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="I21" s="148">
+      <c r="I23" s="146">
         <v>14</v>
       </c>
-      <c r="J21" s="148"/>
-      <c r="K21" s="66" t="s">
+      <c r="J23" s="146"/>
+      <c r="K23" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="L21" s="66"/>
-      <c r="M21" s="126" t="s">
+      <c r="L23" s="66"/>
+      <c r="M23" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="N21" s="59"/>
-    </row>
-    <row r="22" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="57"/>
-      <c r="C22" s="127"/>
-      <c r="D22" s="127"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="127"/>
-      <c r="G22" s="127"/>
-      <c r="H22" s="128" t="s">
+      <c r="N23" s="59"/>
+    </row>
+    <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="57"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="125"/>
+      <c r="F24" s="125"/>
+      <c r="G24" s="125"/>
+      <c r="H24" s="126" t="s">
         <v>118</v>
       </c>
-      <c r="I22" s="188">
+      <c r="I24" s="189">
         <v>14</v>
       </c>
-      <c r="J22" s="188"/>
-      <c r="K22" s="129" t="s">
+      <c r="J24" s="189"/>
+      <c r="K24" s="127" t="s">
         <v>45</v>
       </c>
-      <c r="L22" s="129"/>
-      <c r="M22" s="130" t="s">
+      <c r="L24" s="127"/>
+      <c r="M24" s="128" t="s">
         <v>117</v>
       </c>
-      <c r="N22" s="59"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A23" s="57"/>
-      <c r="B23" s="131"/>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="132"/>
-      <c r="I23" s="133"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="133"/>
-      <c r="N23" s="59"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A24" s="57"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="132"/>
-      <c r="I24" s="133"/>
-      <c r="J24" s="131"/>
-      <c r="K24" s="131"/>
-      <c r="L24" s="131"/>
-      <c r="M24" s="133"/>
       <c r="N24" s="59"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="57"/>
-      <c r="B25" s="131"/>
-      <c r="C25" s="131"/>
-      <c r="D25" s="131"/>
-      <c r="E25" s="131"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
       <c r="F25" s="60"/>
       <c r="G25" s="60"/>
-      <c r="H25" s="132"/>
-      <c r="I25" s="133"/>
-      <c r="J25" s="131"/>
-      <c r="K25" s="131"/>
-      <c r="L25" s="131"/>
-      <c r="M25" s="133"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="131"/>
+      <c r="J25" s="129"/>
+      <c r="K25" s="129"/>
+      <c r="L25" s="129"/>
+      <c r="M25" s="131"/>
       <c r="N25" s="59"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="57"/>
-      <c r="B26" s="131"/>
-      <c r="C26" s="131"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
       <c r="F26" s="60"/>
       <c r="G26" s="60"/>
-      <c r="H26" s="132"/>
-      <c r="I26" s="133"/>
-      <c r="J26" s="131"/>
-      <c r="K26" s="131"/>
-      <c r="L26" s="131"/>
-      <c r="M26" s="133"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="129"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="129"/>
+      <c r="M26" s="131"/>
       <c r="N26" s="59"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="57"/>
-      <c r="B27" s="131"/>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="129"/>
       <c r="F27" s="60"/>
       <c r="G27" s="60"/>
-      <c r="H27" s="132"/>
-      <c r="I27" s="133"/>
-      <c r="J27" s="131"/>
-      <c r="K27" s="131"/>
-      <c r="L27" s="131"/>
-      <c r="M27" s="133"/>
+      <c r="H27" s="130"/>
+      <c r="I27" s="131"/>
+      <c r="J27" s="129"/>
+      <c r="K27" s="129"/>
+      <c r="L27" s="129"/>
+      <c r="M27" s="131"/>
       <c r="N27" s="59"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="57"/>
-      <c r="B28" s="131"/>
-      <c r="C28" s="131"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="131"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="129"/>
       <c r="F28" s="60"/>
       <c r="G28" s="60"/>
-      <c r="H28" s="132"/>
-      <c r="I28" s="133"/>
-      <c r="J28" s="131"/>
-      <c r="K28" s="131"/>
-      <c r="L28" s="131"/>
-      <c r="M28" s="133"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="129"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="129"/>
+      <c r="M28" s="131"/>
       <c r="N28" s="59"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="57"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="131"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
       <c r="F29" s="60"/>
       <c r="G29" s="60"/>
-      <c r="H29" s="132"/>
-      <c r="I29" s="133"/>
-      <c r="J29" s="131"/>
-      <c r="K29" s="131"/>
-      <c r="L29" s="131"/>
-      <c r="M29" s="133"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="129"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="129"/>
+      <c r="M29" s="131"/>
       <c r="N29" s="59"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="57"/>
-      <c r="B30" s="131"/>
-      <c r="C30" s="131"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="131"/>
+      <c r="B30" s="129"/>
+      <c r="C30" s="129"/>
+      <c r="D30" s="129"/>
+      <c r="E30" s="129"/>
       <c r="F30" s="60"/>
       <c r="G30" s="60"/>
-      <c r="H30" s="132"/>
-      <c r="I30" s="133"/>
-      <c r="J30" s="131"/>
-      <c r="K30" s="131"/>
-      <c r="L30" s="131"/>
-      <c r="M30" s="133"/>
+      <c r="H30" s="130"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="129"/>
+      <c r="K30" s="129"/>
+      <c r="L30" s="129"/>
+      <c r="M30" s="131"/>
       <c r="N30" s="59"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="57"/>
-      <c r="B31" s="131"/>
-      <c r="C31" s="131"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="131"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="129"/>
       <c r="F31" s="60"/>
       <c r="G31" s="60"/>
-      <c r="H31" s="132"/>
-      <c r="I31" s="133"/>
-      <c r="J31" s="131"/>
-      <c r="K31" s="131"/>
-      <c r="L31" s="131"/>
-      <c r="M31" s="133"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="131"/>
+      <c r="J31" s="129"/>
+      <c r="K31" s="129"/>
+      <c r="L31" s="129"/>
+      <c r="M31" s="131"/>
       <c r="N31" s="59"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A32" s="57"/>
-      <c r="B32" s="131"/>
-      <c r="C32" s="131"/>
-      <c r="D32" s="131"/>
-      <c r="E32" s="131"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="129"/>
+      <c r="E32" s="129"/>
       <c r="F32" s="60"/>
       <c r="G32" s="60"/>
-      <c r="H32" s="132"/>
-      <c r="I32" s="133"/>
-      <c r="J32" s="131"/>
-      <c r="K32" s="131"/>
-      <c r="L32" s="131"/>
-      <c r="M32" s="133"/>
+      <c r="H32" s="130"/>
+      <c r="I32" s="131"/>
+      <c r="J32" s="129"/>
+      <c r="K32" s="129"/>
+      <c r="L32" s="129"/>
+      <c r="M32" s="131"/>
       <c r="N32" s="59"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="57"/>
-      <c r="B33" s="131"/>
-      <c r="C33" s="131"/>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
       <c r="F33" s="60"/>
       <c r="G33" s="60"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="133"/>
-      <c r="J33" s="131"/>
-      <c r="K33" s="131"/>
-      <c r="L33" s="131"/>
-      <c r="M33" s="133"/>
+      <c r="H33" s="130"/>
+      <c r="I33" s="131"/>
+      <c r="J33" s="129"/>
+      <c r="K33" s="129"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="131"/>
       <c r="N33" s="59"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="57"/>
-      <c r="B34" s="131"/>
-      <c r="C34" s="131"/>
-      <c r="D34" s="131"/>
-      <c r="E34" s="131"/>
+      <c r="B34" s="129"/>
+      <c r="C34" s="129"/>
+      <c r="D34" s="129"/>
+      <c r="E34" s="129"/>
       <c r="F34" s="60"/>
       <c r="G34" s="60"/>
-      <c r="H34" s="132"/>
-      <c r="I34" s="133"/>
-      <c r="J34" s="131"/>
-      <c r="K34" s="131"/>
-      <c r="L34" s="131"/>
-      <c r="M34" s="133"/>
+      <c r="H34" s="130"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="129"/>
+      <c r="K34" s="129"/>
+      <c r="L34" s="129"/>
+      <c r="M34" s="131"/>
       <c r="N34" s="59"/>
     </row>
-    <row r="35" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="57"/>
-      <c r="C35" s="131"/>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="129"/>
       <c r="F35" s="60"/>
       <c r="G35" s="60"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="131"/>
-      <c r="M35" s="65"/>
+      <c r="H35" s="130"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="129"/>
+      <c r="K35" s="129"/>
+      <c r="L35" s="129"/>
+      <c r="M35" s="131"/>
       <c r="N35" s="59"/>
     </row>
-    <row r="36" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="57"/>
-      <c r="B36" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="134"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="134"/>
-      <c r="F36" s="135"/>
-      <c r="G36" s="135"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="137" t="s">
-        <v>119</v>
-      </c>
-      <c r="J36" s="138"/>
-      <c r="K36" s="138"/>
-      <c r="L36" s="138"/>
-      <c r="M36" s="138"/>
+      <c r="B36" s="129"/>
+      <c r="C36" s="129"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="130"/>
+      <c r="I36" s="131"/>
+      <c r="J36" s="129"/>
+      <c r="K36" s="129"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="131"/>
       <c r="N36" s="59"/>
     </row>
-    <row r="37" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="57"/>
-      <c r="B37" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" s="131"/>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
+      <c r="C37" s="129"/>
+      <c r="D37" s="129"/>
+      <c r="E37" s="129"/>
       <c r="F37" s="60"/>
       <c r="G37" s="60"/>
       <c r="H37" s="65"/>
-      <c r="I37" s="139"/>
+      <c r="I37" s="65"/>
       <c r="J37" s="58"/>
       <c r="K37" s="58"/>
-      <c r="L37" s="131"/>
+      <c r="L37" s="129"/>
       <c r="M37" s="65"/>
       <c r="N37" s="59"/>
     </row>
     <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="57"/>
-      <c r="B38" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="131"/>
-      <c r="D38" s="131"/>
-      <c r="E38" s="131"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="139"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="131"/>
-      <c r="M38" s="65"/>
+      <c r="B38" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="133"/>
+      <c r="G38" s="133"/>
+      <c r="H38" s="134"/>
+      <c r="I38" s="135" t="s">
+        <v>119</v>
+      </c>
+      <c r="J38" s="136"/>
+      <c r="K38" s="136"/>
+      <c r="L38" s="136"/>
+      <c r="M38" s="136"/>
       <c r="N38" s="59"/>
     </row>
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="57"/>
       <c r="B39" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="131"/>
-      <c r="D39" s="131"/>
-      <c r="E39" s="131"/>
+        <v>120</v>
+      </c>
+      <c r="C39" s="129"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="129"/>
       <c r="F39" s="60"/>
       <c r="G39" s="60"/>
       <c r="H39" s="65"/>
-      <c r="I39" s="139"/>
+      <c r="I39" s="137"/>
       <c r="J39" s="58"/>
       <c r="K39" s="58"/>
-      <c r="L39" s="131"/>
+      <c r="L39" s="129"/>
       <c r="M39" s="65"/>
       <c r="N39" s="59"/>
     </row>
-    <row r="40" spans="1:14" s="147" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="140"/>
-      <c r="B40" s="62" t="s">
+    <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="57"/>
+      <c r="B40" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="129"/>
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="137"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="129"/>
+      <c r="M40" s="65"/>
+      <c r="N40" s="59"/>
+    </row>
+    <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="57"/>
+      <c r="B41" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="129"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="137"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="129"/>
+      <c r="M41" s="65"/>
+      <c r="N41" s="59"/>
+    </row>
+    <row r="42" spans="1:14" s="145" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="138"/>
+      <c r="B42" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="141"/>
-      <c r="D40" s="141"/>
-      <c r="E40" s="141"/>
-      <c r="F40" s="142"/>
-      <c r="G40" s="142"/>
-      <c r="H40" s="143"/>
-      <c r="I40" s="144"/>
-      <c r="J40" s="145"/>
-      <c r="K40" s="145"/>
-      <c r="L40" s="145"/>
-      <c r="M40" s="145"/>
-      <c r="N40" s="146"/>
-    </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+      <c r="C42" s="139"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="142"/>
+      <c r="J42" s="143"/>
+      <c r="K42" s="143"/>
+      <c r="L42" s="143"/>
+      <c r="M42" s="143"/>
+      <c r="N42" s="144"/>
+    </row>
     <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
@@ -3883,10 +3930,12 @@
     <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="49" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="50" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="51" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I24:J24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
minor bugs in fca export fixed
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_FCA.xlsx
+++ b/templates/Export_Agreement_FCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03124B46-F32F-4024-8422-C0991F048A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D164CE89-E84C-4CCC-9DA8-8415E86A44B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
@@ -815,7 +815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1241,6 +1241,90 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1253,93 +1337,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1751,18 +1752,18 @@
       </c>
     </row>
     <row r="2" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="157" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="177" t="s">
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
       <c r="J2" s="9"/>
       <c r="L2" s="11"/>
       <c r="O2" s="10"/>
@@ -1779,18 +1780,18 @@
       <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="180" t="s">
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1807,18 +1808,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="180" t="s">
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1839,18 +1840,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="163" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="185"/>
-      <c r="F5" s="183" t="s">
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="163" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
+      <c r="G5" s="164"/>
+      <c r="H5" s="164"/>
+      <c r="I5" s="164"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1859,18 +1860,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="161" t="s">
+      <c r="B6" s="166" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="161" t="s">
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="166" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="162"/>
+      <c r="G6" s="167"/>
+      <c r="H6" s="167"/>
+      <c r="I6" s="167"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1915,12 +1916,12 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="186" t="s">
+      <c r="B8" s="169" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="187"/>
-      <c r="D8" s="187"/>
-      <c r="E8" s="188"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="171"/>
       <c r="F8" s="154" t="s">
         <v>10</v>
       </c>
@@ -1973,18 +1974,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="161" t="s">
+      <c r="B11" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="162"/>
-      <c r="D11" s="162"/>
-      <c r="E11" s="163"/>
-      <c r="F11" s="161" t="s">
+      <c r="C11" s="167"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="166" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="162"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="162"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="167"/>
+      <c r="I11" s="167"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2114,18 +2115,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="172"/>
-      <c r="D16" s="172"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="173"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="171" t="s">
+      <c r="F16" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="172"/>
-      <c r="H16" s="172"/>
-      <c r="I16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="174"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2146,15 +2147,15 @@
       <c r="B17" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="174"/>
-      <c r="D17" s="174"/>
-      <c r="E17" s="175"/>
-      <c r="F17" s="176" t="s">
+      <c r="C17" s="175"/>
+      <c r="D17" s="175"/>
+      <c r="E17" s="176"/>
+      <c r="F17" s="177" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="174"/>
-      <c r="H17" s="174"/>
-      <c r="I17" s="174"/>
+      <c r="G17" s="175"/>
+      <c r="H17" s="175"/>
+      <c r="I17" s="175"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2172,16 +2173,16 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="167" t="s">
+      <c r="B18" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="168"/>
-      <c r="D18" s="168"/>
-      <c r="E18" s="168"/>
-      <c r="F18" s="167" t="s">
+      <c r="C18" s="179"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="168"/>
+      <c r="G18" s="179"/>
       <c r="H18" s="23" t="s">
         <v>77</v>
       </c>
@@ -2205,16 +2206,16 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="169" t="s">
+      <c r="B19" s="180" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="170"/>
-      <c r="D19" s="170"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="169" t="s">
+      <c r="C19" s="181"/>
+      <c r="D19" s="181"/>
+      <c r="E19" s="181"/>
+      <c r="F19" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="170"/>
+      <c r="G19" s="181"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2425,12 +2426,12 @@
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="164" t="s">
+      <c r="B27" s="182" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="166"/>
+      <c r="C27" s="183"/>
+      <c r="D27" s="183"/>
+      <c r="E27" s="184"/>
       <c r="F27" s="68" t="s">
         <v>73</v>
       </c>
@@ -2440,18 +2441,18 @@
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="161" t="s">
+      <c r="B28" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="162"/>
-      <c r="D28" s="162"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="161" t="s">
+      <c r="F28" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="162"/>
-      <c r="H28" s="162"/>
-      <c r="I28" s="163"/>
+      <c r="G28" s="167"/>
+      <c r="H28" s="167"/>
+      <c r="I28" s="168"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2487,18 +2488,18 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="161" t="s">
+      <c r="B30" s="166" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="162"/>
-      <c r="D30" s="162"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="161" t="s">
+      <c r="F30" s="166" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="162"/>
-      <c r="H30" s="162"/>
-      <c r="I30" s="163"/>
+      <c r="G30" s="167"/>
+      <c r="H30" s="167"/>
+      <c r="I30" s="168"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2517,18 +2518,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="157" t="s">
+      <c r="B32" s="185" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="157" t="s">
+      <c r="C32" s="186"/>
+      <c r="D32" s="186"/>
+      <c r="E32" s="187"/>
+      <c r="F32" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="158"/>
-      <c r="H32" s="158"/>
-      <c r="I32" s="158"/>
+      <c r="G32" s="186"/>
+      <c r="H32" s="186"/>
+      <c r="I32" s="186"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2654,18 +2655,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="157" t="s">
+      <c r="B40" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="158"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="159"/>
-      <c r="F40" s="157" t="s">
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="187"/>
+      <c r="F40" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="160"/>
-      <c r="H40" s="160"/>
-      <c r="I40" s="160"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2987,6 +2988,51 @@
     <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="F46:I46"/>
     <mergeCell ref="B2:E2"/>
@@ -3003,51 +3049,6 @@
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <conditionalFormatting sqref="F19 J19 B20:E20 I20:J22 B21:B22 E21:E22">
     <cfRule type="notContainsBlanks" dxfId="3" priority="1">
@@ -3087,7 +3088,7 @@
   <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3490,7 +3491,7 @@
       <c r="E19" s="106"/>
       <c r="F19" s="112"/>
       <c r="G19" s="104"/>
-      <c r="H19" s="91" t="s">
+      <c r="H19" s="190" t="s">
         <v>125</v>
       </c>
       <c r="I19" s="106"/>
@@ -3510,7 +3511,7 @@
       <c r="E20" s="106"/>
       <c r="F20" s="112"/>
       <c r="G20" s="104"/>
-      <c r="H20" s="84" t="s">
+      <c r="H20" s="86" t="s">
         <v>45</v>
       </c>
       <c r="I20" s="106"/>

</xml_diff>